<commit_message>
update view main page
</commit_message>
<xml_diff>
--- a/view_plan.xlsx
+++ b/view_plan.xlsx
@@ -184,60 +184,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>47626</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>44</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="正方形/長方形 4"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="933450" y="2276476"/>
-          <a:ext cx="7172325" cy="1171574"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>104775</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -285,6 +231,244 @@
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>投票</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="テキスト ボックス 6"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1190625" y="2171700"/>
+          <a:ext cx="3286125" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
+            <a:t>投票を作成する</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="テキスト ボックス 7"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1190625" y="3152775"/>
+          <a:ext cx="3286125" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>投票</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="テキスト ボックス 8"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4629150" y="3152775"/>
+          <a:ext cx="3286125" cy="2533650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>投票</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="テキスト ボックス 9"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648200" y="2171700"/>
+          <a:ext cx="3286125" cy="476250"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
         </a:fontRef>
       </xdr:style>
       <xdr:txBody>
@@ -592,7 +776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="BA8" sqref="BA8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update survey column update views
</commit_message>
<xml_diff>
--- a/view_plan.xlsx
+++ b/view_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355"/>
   </bookViews>
   <sheets>
     <sheet name="all_page_view" sheetId="6" r:id="rId1"/>
@@ -938,7 +938,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>create</a:t>
+            <a:t>make</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
         </a:p>
@@ -1344,6 +1344,117 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
+    <dgm:pt modelId="{629E773C-EE7D-482A-94D1-6BB3211F734D}">
+      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>check</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" type="parTrans" cxnId="{EED1F78C-85BA-4908-9EDB-040048925EE2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D18382C1-3316-401F-B9F7-5740273EBE35}" type="sibTrans" cxnId="{EED1F78C-85BA-4908-9EDB-040048925EE2}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9019F039-A6BB-4811-9BF3-881F48EB4453}">
+      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" type="parTrans" cxnId="{1103E670-28FF-4AB2-9FAA-8999DB660777}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0F39B1C9-85F1-4DD3-8B99-1EDD809C502C}" type="sibTrans" cxnId="{1103E670-28FF-4AB2-9FAA-8999DB660777}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}">
+      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>end</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" type="parTrans" cxnId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}" type="sibTrans" cxnId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
     <dgm:pt modelId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" type="pres">
       <dgm:prSet presAssocID="{0AACF41D-7981-4393-B317-C2E0308F1883}" presName="hierChild1" presStyleCnt="0">
         <dgm:presLayoutVars>
@@ -1460,7 +1571,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" type="pres">
-      <dgm:prSet presAssocID="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1483,7 +1594,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" type="pres">
-      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="4">
+      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="7">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1498,7 +1609,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" type="pres">
-      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1517,7 +1628,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" type="pres">
-      <dgm:prSet presAssocID="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1540,7 +1651,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" type="pres">
-      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="4">
+      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="7">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1555,7 +1666,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" type="pres">
-      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1630,6 +1741,156 @@
       <dgm:prSet presAssocID="{82F277AB-87C7-433B-862F-87C13847027E}" presName="hierChild4" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
+    <dgm:pt modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" type="pres">
+      <dgm:prSet presAssocID="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{83391BB5-AFDB-487B-8E65-A8933F5D40C0}" type="pres">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{CE268437-5864-494B-97A2-F73F1BE94CBB}" type="pres">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" type="pres">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootText" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" type="pres">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="7"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{07FD2249-CC06-4FCC-BFDD-5DAB1864547E}" type="pres">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3687E432-C064-468F-A8F9-61357CB3CA04}" type="pres">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{224BDC60-7934-422F-B29C-84F028B56716}" type="pres">
+      <dgm:prSet presAssocID="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{02B42FDE-E435-4D7F-BCA4-7B0F81D6BEE7}" type="pres">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C5CA1F46-EAD5-4E54-A72E-2D795B66C7B5}" type="pres">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" type="pres">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootText" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" type="pres">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="7"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C8647CEA-EBF2-4C35-8253-BD95D471C3AC}" type="pres">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{CE18ECFC-CD43-41B2-88A2-2F1E8E86FD7C}" type="pres">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" type="pres">
+      <dgm:prSet presAssocID="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1CF3CCC9-8575-45C6-8D49-050F1EF2260B}" type="pres">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B31D51FC-E76F-4E0B-BBB2-388F639045E3}" type="pres">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" type="pres">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootText" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" type="pres">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="7"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{7FC98DE9-0185-407D-B6C9-73AF55C9EE0D}" type="pres">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0E4330CF-7ACC-4689-B989-4C3902DD4AFD}" type="pres">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
     <dgm:pt modelId="{FE57FF36-DCE8-4FFF-9AC7-AC9F89208209}" type="pres">
       <dgm:prSet presAssocID="{82F277AB-87C7-433B-862F-87C13847027E}" presName="hierChild5" presStyleCnt="0"/>
       <dgm:spPr/>
@@ -1745,7 +2006,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" type="pres">
-      <dgm:prSet presAssocID="{CC820015-08D8-4836-A31C-2D63FBA54C31}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{CC820015-08D8-4836-A31C-2D63FBA54C31}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1768,7 +2029,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" type="pres">
-      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootText" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="4">
+      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootText" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="7">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1783,7 +2044,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" type="pres">
-      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1802,7 +2063,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" type="pres">
-      <dgm:prSet presAssocID="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1825,7 +2086,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}" type="pres">
-      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootText" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="4">
+      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootText" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="7">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1840,7 +2101,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8D67E224-0EDF-448A-9790-7C530F95D644}" type="pres">
-      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="4"/>
+      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="7"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2039,54 +2300,66 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{A0BA6098-4B55-4BA5-B458-EABF50C624B8}" type="presOf" srcId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{4E77CAF1-AB7F-4789-9D33-7ACC3ED65CAC}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{0FAB1775-08F8-482E-A204-647B49CA8593}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{559ADFF3-0478-496C-AFD5-D9545B790EC4}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FA5FD46B-9D83-45A4-9344-56D6066107F5}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1B7EE4ED-C343-4DBF-8592-DAF824F32B4F}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{5AD42C2B-3B72-4332-8CB0-CB02483CBB7A}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{0A3BCE5E-23D3-4914-A0DE-4D82B34706DE}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" srcOrd="0" destOrd="0" parTransId="{CCD73AB5-5FAC-49DE-B051-A16352DE18B0}" sibTransId="{90EBE641-EF69-4D14-98EF-9FFC06AA100B}"/>
+    <dgm:cxn modelId="{6B143136-E6DE-46E8-9AD5-1977D53BF989}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{0FAB1775-08F8-482E-A204-647B49CA8593}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{320201D6-8AE1-4176-9635-D81197B9E8AD}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1103E670-28FF-4AB2-9FAA-8999DB660777}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" srcOrd="1" destOrd="0" parTransId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" sibTransId="{0F39B1C9-85F1-4DD3-8B99-1EDD809C502C}"/>
+    <dgm:cxn modelId="{6DB29CA3-84E3-4AE3-B269-0E4E9A2370AB}" type="presOf" srcId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" destId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{41EA2324-B53B-4930-BACB-AFDEA8715A7A}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{215983E4-081D-4467-A756-55FEF443A562}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{815260D8-FCB5-45E3-8AFB-F460679B2CDE}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{63A697A5-BE9C-4F91-A92C-3506C14F0A22}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2415E457-D5E9-475F-B3CE-4993C41B9B2A}" type="presOf" srcId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" destId="{9451D74F-6692-4FF1-A580-5574CD4401DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{32C55363-4473-460E-A765-20AB775E2E35}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{EED1F78C-85BA-4908-9EDB-040048925EE2}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" srcOrd="0" destOrd="0" parTransId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" sibTransId="{D18382C1-3316-401F-B9F7-5740273EBE35}"/>
+    <dgm:cxn modelId="{752DC3CA-1459-43DF-8D17-59075C9B7B68}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{83B3D6F2-C63A-4120-828B-5A15440C2D24}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D01C7126-32B6-4DB4-833B-0C12061AE485}" type="presOf" srcId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" destId="{224BDC60-7934-422F-B29C-84F028B56716}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FC7B3FFE-23C2-480C-9156-521BA5E4ED21}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{B7442801-F217-4912-AE49-8224D444B7AE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{47E9E0D7-561B-4062-99B9-8E5422CA1060}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{404FFDC8-1807-40B1-88B3-D52B6630D710}" type="presOf" srcId="{CEED879D-C918-490C-A079-5102097205A7}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FE9E3000-93A4-4B79-A18F-D60B82D46552}" type="presOf" srcId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{BEE184DB-6F27-4D7A-9C18-98A0A01EDA70}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7BDC27E4-38E1-44C6-9275-7D0DAB391DBF}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D8ED3677-8BE0-47AD-826F-58E9D454D3D0}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" srcOrd="2" destOrd="0" parTransId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" sibTransId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}"/>
+    <dgm:cxn modelId="{33CBFE4F-047C-4EDF-8FBC-62953BACFD7B}" type="presOf" srcId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" destId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7AC678BE-C1B9-4C2C-BBA5-63C6027EC514}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{35A1554D-6075-49F2-94F5-D41A56B41CB3}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{DC212456-5040-4495-9F5E-3AA3C3560C20}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B9E26008-760E-4F53-A157-28E1F48ABE00}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" srcOrd="0" destOrd="0" parTransId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" sibTransId="{0F0D26FC-9E72-450A-A689-3301417EC882}"/>
+    <dgm:cxn modelId="{DE057FFD-529A-4E2E-B498-BC5F7742815B}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{078BFD8E-7E7A-44CB-8C2A-862AA6B7EF64}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D823C5EF-1423-4863-AAC0-3CCB22E52AE5}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" srcOrd="0" destOrd="0" parTransId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" sibTransId="{EA4D083E-0312-47CC-8039-9496D55CDBDC}"/>
+    <dgm:cxn modelId="{E929C590-2797-4F5F-A36A-48FC41BCAC3F}" type="presOf" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{3F8AEC38-DCAC-422E-BBE1-60F8D32065DD}" type="presOf" srcId="{16684A72-88D1-4068-9742-A287A1AF7991}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{97FB1D32-8AB3-45A8-8D63-292929166F76}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" srcOrd="1" destOrd="0" parTransId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" sibTransId="{2AD778EF-0F85-4883-B9FB-FEB9810673D5}"/>
+    <dgm:cxn modelId="{38BB76FF-0FA4-4F6D-A1F3-00F631A74DDB}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" srcOrd="3" destOrd="0" parTransId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" sibTransId="{DA3E9CE7-349A-4E9E-BD8A-D3E3EE2D990C}"/>
+    <dgm:cxn modelId="{AD187AFA-F1B3-417B-A18B-1DA461641B00}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2135CB57-A821-4A45-B869-6D0CF021FCED}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" srcOrd="4" destOrd="0" parTransId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" sibTransId="{49B5EA05-D380-4B41-9D7A-E2087005D6BD}"/>
+    <dgm:cxn modelId="{BB4B00DC-A343-4429-9992-C97EBA76F0AA}" type="presOf" srcId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E1971364-B9C9-4F2D-8D2C-1C3FFC969523}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" srcOrd="2" destOrd="0" parTransId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" sibTransId="{12ED1614-9395-4694-B66E-BE7517C9B3C3}"/>
+    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="1" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
+    <dgm:cxn modelId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" srcOrd="6" destOrd="0" parTransId="{CEED879D-C918-490C-A079-5102097205A7}" sibTransId="{96D318EA-92A6-4D06-8BD0-F3437FB33BA9}"/>
     <dgm:cxn modelId="{F30AFEB2-A830-4035-BA71-EB491C42489C}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" srcOrd="0" destOrd="0" parTransId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" sibTransId="{E8DF5D1F-4EAF-4749-95FB-4BF5DDF36D94}"/>
-    <dgm:cxn modelId="{0A4144C8-2D15-4938-8E46-FC9DD289F65E}" type="presOf" srcId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{1F92A6FB-9181-483A-92B2-3C4BA191B8AC}" type="presOf" srcId="{CEED879D-C918-490C-A079-5102097205A7}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{94E018CE-E921-407B-A6D7-074FD16D89BD}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{13D64C26-9E69-4757-8283-81A9EE7A80CD}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{28369DE3-437A-4135-B55E-48F1D6296DC6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E929C590-2797-4F5F-A36A-48FC41BCAC3F}" type="presOf" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{B9E26008-760E-4F53-A157-28E1F48ABE00}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" srcOrd="0" destOrd="0" parTransId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" sibTransId="{0F0D26FC-9E72-450A-A689-3301417EC882}"/>
+    <dgm:cxn modelId="{0B25676A-30F3-4EC1-A0B7-586CBD08E376}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{28369DE3-437A-4135-B55E-48F1D6296DC6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{442C35E7-9219-42B1-8589-CA6B5AFD7FD1}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" srcOrd="5" destOrd="0" parTransId="{16684A72-88D1-4068-9742-A287A1AF7991}" sibTransId="{E1FF0606-7FA7-4C21-8E5B-4C259D042C61}"/>
+    <dgm:cxn modelId="{71DBFE96-B81B-465F-9F92-6E34F83D6304}" type="presOf" srcId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{38DBDA98-E1B6-4DF0-B945-0EC585B5EFB9}" type="presOf" srcId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" destId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E77DC00F-1DBC-4305-A75A-CA0AF88B6519}" type="presOf" srcId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" destId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9F01A4C8-FCDC-41BC-898B-747FEC5B6389}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B0C83AA9-272C-4A44-AC90-24DE78B5CC49}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1117B828-D277-43FA-B244-6FF95B68193E}" type="presOf" srcId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F5EBD142-F152-4BD8-AE52-4066178EEE6D}" type="presOf" srcId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{56247623-20AE-45E9-A8C5-000B0DE85F7F}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{82F277AB-87C7-433B-862F-87C13847027E}" srcOrd="1" destOrd="0" parTransId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" sibTransId="{8C3C1181-DF4B-4EE3-9ED3-562C8BC3A0A0}"/>
+    <dgm:cxn modelId="{814C55A4-746A-46AC-B71C-48916393BAC3}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{F5B18884-E498-499B-92AD-14DA40157B0A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D0A170FC-0AB5-4AEF-91B1-1D414CCEFE41}" type="presOf" srcId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{92107E38-7630-470C-9791-C19A37DEC9FA}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{B2A681BD-5EE0-45B6-B4F9-016D77485296}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{35A1554D-6075-49F2-94F5-D41A56B41CB3}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E77DC00F-1DBC-4305-A75A-CA0AF88B6519}" type="presOf" srcId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" destId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{320201D6-8AE1-4176-9635-D81197B9E8AD}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{2415E457-D5E9-475F-B3CE-4993C41B9B2A}" type="presOf" srcId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" destId="{9451D74F-6692-4FF1-A580-5574CD4401DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{0A8C17FB-D189-4FA8-B487-6BC08BE16983}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{52289317-D528-4C97-8F23-79400B542547}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{442C35E7-9219-42B1-8589-CA6B5AFD7FD1}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" srcOrd="5" destOrd="0" parTransId="{16684A72-88D1-4068-9742-A287A1AF7991}" sibTransId="{E1FF0606-7FA7-4C21-8E5B-4C259D042C61}"/>
-    <dgm:cxn modelId="{D823C5EF-1423-4863-AAC0-3CCB22E52AE5}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" srcOrd="0" destOrd="0" parTransId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" sibTransId="{EA4D083E-0312-47CC-8039-9496D55CDBDC}"/>
-    <dgm:cxn modelId="{7F19E608-9FF6-4617-901B-F116C2C1F248}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{56247623-20AE-45E9-A8C5-000B0DE85F7F}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{82F277AB-87C7-433B-862F-87C13847027E}" srcOrd="1" destOrd="0" parTransId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" sibTransId="{8C3C1181-DF4B-4EE3-9ED3-562C8BC3A0A0}"/>
-    <dgm:cxn modelId="{CA9D5F0F-2169-4C3C-BEAD-3657C2B9E19B}" type="presOf" srcId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E1971364-B9C9-4F2D-8D2C-1C3FFC969523}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" srcOrd="2" destOrd="0" parTransId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" sibTransId="{12ED1614-9395-4694-B66E-BE7517C9B3C3}"/>
-    <dgm:cxn modelId="{BEE184DB-6F27-4D7A-9C18-98A0A01EDA70}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{47E9E0D7-561B-4062-99B9-8E5422CA1060}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{8638B5D1-B30A-4EFD-80C0-2B16792EC4EB}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{F5B18884-E498-499B-92AD-14DA40157B0A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{54A4F72D-9544-4BB7-AAB5-DA8A66EC57EA}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" srcOrd="6" destOrd="0" parTransId="{CEED879D-C918-490C-A079-5102097205A7}" sibTransId="{96D318EA-92A6-4D06-8BD0-F3437FB33BA9}"/>
-    <dgm:cxn modelId="{4ECC1468-EF38-4F16-8772-6DBB5F6EB61D}" type="presOf" srcId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{22B2D994-9A59-44AC-9D27-8517B6C453F8}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{0A3BCE5E-23D3-4914-A0DE-4D82B34706DE}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" srcOrd="0" destOrd="0" parTransId="{CCD73AB5-5FAC-49DE-B051-A16352DE18B0}" sibTransId="{90EBE641-EF69-4D14-98EF-9FFC06AA100B}"/>
-    <dgm:cxn modelId="{97FB1D32-8AB3-45A8-8D63-292929166F76}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" srcOrd="1" destOrd="0" parTransId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" sibTransId="{2AD778EF-0F85-4883-B9FB-FEB9810673D5}"/>
-    <dgm:cxn modelId="{752DC3CA-1459-43DF-8D17-59075C9B7B68}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E6D704B0-C370-4218-9E90-54832F27F333}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{FC7B3FFE-23C2-480C-9156-521BA5E4ED21}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{B7442801-F217-4912-AE49-8224D444B7AE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{08210D7B-C999-4D26-8CBD-3895B53E6AC5}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{33CBFE4F-047C-4EDF-8FBC-62953BACFD7B}" type="presOf" srcId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" destId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D67A248A-80EA-4055-B29D-45173AB80E54}" type="presOf" srcId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{38BB76FF-0FA4-4F6D-A1F3-00F631A74DDB}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" srcOrd="3" destOrd="0" parTransId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" sibTransId="{DA3E9CE7-349A-4E9E-BD8A-D3E3EE2D990C}"/>
-    <dgm:cxn modelId="{5AD42C2B-3B72-4332-8CB0-CB02483CBB7A}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{2135CB57-A821-4A45-B869-6D0CF021FCED}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" srcOrd="4" destOrd="0" parTransId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" sibTransId="{49B5EA05-D380-4B41-9D7A-E2087005D6BD}"/>
-    <dgm:cxn modelId="{178C325B-7A7B-4BE5-8525-690776DB5835}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="1" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
-    <dgm:cxn modelId="{D76ADCC5-C63C-4051-B801-389BC44090F5}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F5EBD142-F152-4BD8-AE52-4066178EEE6D}" type="presOf" srcId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{7BDC27E4-38E1-44C6-9275-7D0DAB391DBF}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{DE057FFD-529A-4E2E-B498-BC5F7742815B}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{078BFD8E-7E7A-44CB-8C2A-862AA6B7EF64}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{38544823-0EE7-4CAF-BE41-6B5104DE34B5}" type="presOf" srcId="{16684A72-88D1-4068-9742-A287A1AF7991}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{3A8D4DF3-E699-49C7-9251-0A31EBDC947E}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1C6CD132-06CD-4B2C-8DDD-553AE71D597C}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7B55AD7D-CC95-45FE-BCFE-7B483051B4CB}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{2D7F7C22-ADD5-4E45-A535-C589EB253F20}" type="presParOf" srcId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" destId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{C9F10509-5022-4B9B-A341-CC3365CCCF88}" type="presParOf" srcId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" destId="{87B98112-BB49-47E9-92F1-82F9448578BD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{CDA112DB-C227-483A-BA50-1640272F1F9E}" type="presParOf" srcId="{87B98112-BB49-47E9-92F1-82F9448578BD}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2119,56 +2392,77 @@
     <dgm:cxn modelId="{57A03B30-FF79-443F-A355-3FF9F6EE22BF}" type="presParOf" srcId="{71DEA10E-FEB7-4A5C-AB9F-215C3F039090}" destId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{0FC10D23-CE6B-401D-B890-0D447DBBE36F}" type="presParOf" srcId="{71DEA10E-FEB7-4A5C-AB9F-215C3F039090}" destId="{B2A681BD-5EE0-45B6-B4F9-016D77485296}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{8C002F93-4D06-4235-B85A-F85D2D7ED52B}" type="presParOf" srcId="{18FF3CE7-B60E-4AE3-8F7D-A95172BC91B6}" destId="{362074D3-FDB9-43CB-ACC0-E86DDDCFFF6D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{ABAA1F13-41D8-45A0-B126-B8CAE329C1C8}" type="presParOf" srcId="{362074D3-FDB9-43CB-ACC0-E86DDDCFFF6D}" destId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{04F7151E-A29F-465A-BA6E-C0A8F5D821EF}" type="presParOf" srcId="{362074D3-FDB9-43CB-ACC0-E86DDDCFFF6D}" destId="{83391BB5-AFDB-487B-8E65-A8933F5D40C0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{18E0053B-F301-45E3-8E8A-78B3C875BFBF}" type="presParOf" srcId="{83391BB5-AFDB-487B-8E65-A8933F5D40C0}" destId="{CE268437-5864-494B-97A2-F73F1BE94CBB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B88CF940-1126-4790-A666-485DF5103F7A}" type="presParOf" srcId="{CE268437-5864-494B-97A2-F73F1BE94CBB}" destId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{DD3DDEDD-DACD-4571-B6F9-19923CB6742C}" type="presParOf" srcId="{CE268437-5864-494B-97A2-F73F1BE94CBB}" destId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9E17CE69-0699-4196-BCDA-DF4E683BD5CB}" type="presParOf" srcId="{83391BB5-AFDB-487B-8E65-A8933F5D40C0}" destId="{07FD2249-CC06-4FCC-BFDD-5DAB1864547E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1FCD826F-BE8D-4156-8630-F8BBE49AF713}" type="presParOf" srcId="{83391BB5-AFDB-487B-8E65-A8933F5D40C0}" destId="{3687E432-C064-468F-A8F9-61357CB3CA04}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2125BC13-3736-4B6C-AF0B-26F7F33A75CA}" type="presParOf" srcId="{362074D3-FDB9-43CB-ACC0-E86DDDCFFF6D}" destId="{224BDC60-7934-422F-B29C-84F028B56716}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F1659140-9641-40A9-9AD5-FFE1ADF75B62}" type="presParOf" srcId="{362074D3-FDB9-43CB-ACC0-E86DDDCFFF6D}" destId="{02B42FDE-E435-4D7F-BCA4-7B0F81D6BEE7}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{04C76861-3657-4A2A-9916-008DA2CCF070}" type="presParOf" srcId="{02B42FDE-E435-4D7F-BCA4-7B0F81D6BEE7}" destId="{C5CA1F46-EAD5-4E54-A72E-2D795B66C7B5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2AC7F896-EB1B-44B1-9ACA-14D2EDB142F7}" type="presParOf" srcId="{C5CA1F46-EAD5-4E54-A72E-2D795B66C7B5}" destId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B0CD4AD4-7E04-45AB-8526-8E17DEC0E4C0}" type="presParOf" srcId="{C5CA1F46-EAD5-4E54-A72E-2D795B66C7B5}" destId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{79B18165-07FF-4C61-8F9C-D77ED9740878}" type="presParOf" srcId="{02B42FDE-E435-4D7F-BCA4-7B0F81D6BEE7}" destId="{C8647CEA-EBF2-4C35-8253-BD95D471C3AC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{CB9261C6-030D-485B-B140-160C04E6D3E8}" type="presParOf" srcId="{02B42FDE-E435-4D7F-BCA4-7B0F81D6BEE7}" destId="{CE18ECFC-CD43-41B2-88A2-2F1E8E86FD7C}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E27E8853-B5A5-4CC3-977D-CD9A39BF32C5}" type="presParOf" srcId="{362074D3-FDB9-43CB-ACC0-E86DDDCFFF6D}" destId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{5B778660-2B11-4575-BFFD-3BB9BE548030}" type="presParOf" srcId="{362074D3-FDB9-43CB-ACC0-E86DDDCFFF6D}" destId="{1CF3CCC9-8575-45C6-8D49-050F1EF2260B}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{AB202F7F-485D-48A9-8DE8-19A048F1642A}" type="presParOf" srcId="{1CF3CCC9-8575-45C6-8D49-050F1EF2260B}" destId="{B31D51FC-E76F-4E0B-BBB2-388F639045E3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{EB795410-2AF1-4F2F-8F83-50B1DBBBFA29}" type="presParOf" srcId="{B31D51FC-E76F-4E0B-BBB2-388F639045E3}" destId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{359ED589-285F-4C96-BC01-5C3ACDD3C3A2}" type="presParOf" srcId="{B31D51FC-E76F-4E0B-BBB2-388F639045E3}" destId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2AD529EB-355E-438B-99FF-6230DBF392F1}" type="presParOf" srcId="{1CF3CCC9-8575-45C6-8D49-050F1EF2260B}" destId="{7FC98DE9-0185-407D-B6C9-73AF55C9EE0D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{CC81FEE7-E22B-4A8A-A3B4-A0849FC8B58C}" type="presParOf" srcId="{1CF3CCC9-8575-45C6-8D49-050F1EF2260B}" destId="{0E4330CF-7ACC-4689-B989-4C3902DD4AFD}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{1F6BA783-6F85-4D7A-B980-FFB4F582E6AD}" type="presParOf" srcId="{18FF3CE7-B60E-4AE3-8F7D-A95172BC91B6}" destId="{FE57FF36-DCE8-4FFF-9AC7-AC9F89208209}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{3AB8DA30-1750-4F26-BA92-FC9AE55B6CB8}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{DDC08525-D63E-4507-83D0-FB215C4E4B87}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{84DCBCBB-8865-466D-8B4C-02DE30AC61E8}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{3CFC457C-A1DB-4EA8-AE0E-A938C364F07C}" type="presParOf" srcId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{31FA92C4-53C0-4C10-A63A-5931E32EA812}" type="presParOf" srcId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F997FDD0-1C2F-48ED-A080-443CBE64F3DC}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{CF2FCF6C-326F-4DC9-B8A1-0BF6C9D81E44}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{5DB2FD0A-5BE2-4785-97D3-44FDE5DF5769}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{0179D0B3-6350-4D61-9B67-663CD880CA02}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{99170F8E-EFAE-4A98-8FD6-4214991E99DD}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{6565F9F1-1ACB-4243-B35A-79A39EEA7674}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F1F0255B-744B-4CED-A6F8-3B841FA0D435}" type="presParOf" srcId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" destId="{58334D2C-E8F3-4882-92A8-711D1F141773}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{8BA4A18B-E321-40D9-BF84-C41A7514881B}" type="presParOf" srcId="{58334D2C-E8F3-4882-92A8-711D1F141773}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F4EFBD0A-8AE6-47B1-8383-02971E36480A}" type="presParOf" srcId="{58334D2C-E8F3-4882-92A8-711D1F141773}" destId="{28369DE3-437A-4135-B55E-48F1D6296DC6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{48107E63-5AED-42EE-8C27-FBCA1EB28C42}" type="presParOf" srcId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" destId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{7A7A6F58-3AF2-4C24-BA44-968BCD2FD423}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{BA60FE16-4FEC-4FE4-9AD8-C1E9C11640FB}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F70CFA57-5A00-4EC9-91EF-57FAFF712C58}" type="presParOf" srcId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" destId="{7AD819AF-DC71-4F6D-B4E4-24C768F7F329}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{4E9D65D0-610E-49A7-BB13-CDC5A8A2F026}" type="presParOf" srcId="{7AD819AF-DC71-4F6D-B4E4-24C768F7F329}" destId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{0BD7C98E-0743-4EDE-9881-14018B0DA056}" type="presParOf" srcId="{7AD819AF-DC71-4F6D-B4E4-24C768F7F329}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{ADE2EF55-FFBF-42FE-8937-219D9B23FE24}" type="presParOf" srcId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" destId="{2383EC66-011C-464A-AE9E-B8EF60E71009}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{938B2183-443B-4830-BD1A-BC1188B04A50}" type="presParOf" srcId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" destId="{3FB70AC5-DA95-40D9-808D-7DBDFAF5AD48}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{DE50E24A-3042-4DB5-971C-655F787572DC}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{62479691-35C5-4DD9-9465-1EE18E0B6790}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AE035E31-79A2-4B8D-81C1-52266F2215B6}" type="presParOf" srcId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" destId="{0F8A7C2B-1759-4FB3-8042-677439E48219}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{8CB47FE8-9E3F-4113-8972-6E825CFA5889}" type="presParOf" srcId="{0F8A7C2B-1759-4FB3-8042-677439E48219}" destId="{F5B18884-E498-499B-92AD-14DA40157B0A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{BAF1DDE1-C741-491A-A364-D2CBFBC7A655}" type="presParOf" srcId="{0F8A7C2B-1759-4FB3-8042-677439E48219}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{3957A738-C501-473B-8E20-A1CD39AD9DE8}" type="presParOf" srcId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" destId="{323A9B1A-E968-47F7-BED6-41A759F568C3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{6307AB6F-FC5D-4606-A04E-2E8EECAD6CEC}" type="presParOf" srcId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" destId="{34F96038-D67A-46A4-B7CA-55B5FE28E7CF}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{12459FD4-EC3C-47F1-BF7C-9FF858AFA5BF}" type="presParOf" srcId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" destId="{25801B8D-95D6-48CD-93F1-3025ED251512}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{8EE391A4-9457-44B1-9930-8002EA0FBE84}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{BABA2028-7774-4190-BD4E-46E8B30346C6}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{023D105C-727F-4B80-853C-64AB2A0F3749}" srcOrd="9" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{4F1E82C8-BF97-4E97-A03F-8BDA57A04DF6}" type="presParOf" srcId="{023D105C-727F-4B80-853C-64AB2A0F3749}" destId="{8BC333C7-7439-44E7-B907-DB6755839F28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D5C3927A-FDE3-4CBF-99B2-773200739F9E}" type="presParOf" srcId="{8BC333C7-7439-44E7-B907-DB6755839F28}" destId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{0B1E0689-9675-4651-A4B3-052CB9208AB0}" type="presParOf" srcId="{8BC333C7-7439-44E7-B907-DB6755839F28}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{471157FB-E02E-47B0-B682-AF77DA529669}" type="presParOf" srcId="{023D105C-727F-4B80-853C-64AB2A0F3749}" destId="{25BB545E-6C6F-4D7E-AC44-1F23E3318EF9}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{970ECC28-EEF5-4110-94C6-454DB3515862}" type="presParOf" srcId="{023D105C-727F-4B80-853C-64AB2A0F3749}" destId="{E63BC231-8990-4828-933B-663A84A923E7}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{ADE2E45C-A368-4ABA-BC64-76A19A5EE8DC}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="10" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F9FD872F-0109-4A83-8C05-C7805A1431B3}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{14920BCF-0F77-45F3-AF09-5773FB403370}" srcOrd="11" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E5C90614-0278-4E89-9CA0-F4DDF79B80E9}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{951A5EBE-973F-49D2-AEE8-E9C1FD21E621}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D4BF82DB-C59B-4E72-AC50-AF792682F072}" type="presParOf" srcId="{951A5EBE-973F-49D2-AEE8-E9C1FD21E621}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{10339933-44EB-42EB-BF33-D1EB946070C0}" type="presParOf" srcId="{951A5EBE-973F-49D2-AEE8-E9C1FD21E621}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{07998C37-45FF-4661-ACB9-ECF3401CBAA8}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{5154CB22-61FB-414C-948D-B5CAB376CD6A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{15F08C7B-E254-4910-8BD5-FD81FD01C885}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{E0CF165D-444F-4D0C-9894-0CEE601662E0}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{5190EA15-3921-4CFB-AFB1-C123E064D7B2}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="12" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{49B4F40E-364C-41C1-A871-4D8EDCAE1AD7}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" srcOrd="13" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{30D47C6B-A8F0-4581-815B-A7432DF412F7}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{01CFBFF8-8D53-4041-998A-732E150B2CFA}" type="presParOf" srcId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" destId="{0FAB1775-08F8-482E-A204-647B49CA8593}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{B5344E4B-7C1F-4687-AD6B-F7CB7F56FF77}" type="presParOf" srcId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{31823A86-AAE2-4BC4-A85E-CA7ED59E1296}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{4AEBA50B-F3AB-455F-808A-6D8D6F6C8FC7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{B9004EFE-5C83-46CD-9C78-561792BA8A1B}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{47D9F871-9894-4842-A60A-C9A1F58C3CB5}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{46E81D77-740D-484D-9A4C-98E0C5DC3EF3}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{26169FCB-909B-4991-B2F2-9D496304DF92}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6D4786D0-0FEB-480E-9ACB-0B0EFB5F31C9}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E977C6FF-7906-45F1-903A-F572CE9B3D3B}" type="presParOf" srcId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{234AC40D-7A12-4A42-8747-1718EA8724EF}" type="presParOf" srcId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{82A5785E-3DD7-4D75-84AE-00C846E6CA34}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{CF2FCF6C-326F-4DC9-B8A1-0BF6C9D81E44}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{49DD7261-B542-4333-BBCD-7F647314647E}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{0179D0B3-6350-4D61-9B67-663CD880CA02}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7DBE53AB-4C21-483C-A0DF-B2FDF0DDEA0C}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{0D9B4DB5-A00D-4982-89A0-AD4E75620233}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{BADF57DC-8835-4928-9107-E2C3C4EDEA7F}" type="presParOf" srcId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" destId="{58334D2C-E8F3-4882-92A8-711D1F141773}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{EA80DEC0-C846-4C3E-86CF-2A07527F7551}" type="presParOf" srcId="{58334D2C-E8F3-4882-92A8-711D1F141773}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9E577B9A-B581-43C3-A21A-C6BC4CFAA82F}" type="presParOf" srcId="{58334D2C-E8F3-4882-92A8-711D1F141773}" destId="{28369DE3-437A-4135-B55E-48F1D6296DC6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{CE8B979D-0A2D-401C-A5DA-ED2967720303}" type="presParOf" srcId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" destId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7898F52B-7358-49EC-BFFF-A7787977C98D}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{45A8AD2F-6B73-479C-BD79-8915FBE7AB07}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{70A44B34-BE6F-4186-900C-158A29F5B981}" type="presParOf" srcId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" destId="{7AD819AF-DC71-4F6D-B4E4-24C768F7F329}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{3AD81C77-3B56-466E-81AF-47C01BBB923A}" type="presParOf" srcId="{7AD819AF-DC71-4F6D-B4E4-24C768F7F329}" destId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2DC5ED20-6B5A-44A9-B02A-9E00DE14FEB0}" type="presParOf" srcId="{7AD819AF-DC71-4F6D-B4E4-24C768F7F329}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{87D4347F-CB73-47AF-8660-5FE8EF1E758E}" type="presParOf" srcId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" destId="{2383EC66-011C-464A-AE9E-B8EF60E71009}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{EA07903E-53D5-4622-B150-6CDE2F133776}" type="presParOf" srcId="{D35DA0C1-4C7F-4AE6-9326-9CC65C903CFC}" destId="{3FB70AC5-DA95-40D9-808D-7DBDFAF5AD48}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B9A226A5-6B88-4AC1-AF4E-97F42888F308}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{21F677FF-96A0-4BE4-8813-3291A496496F}" type="presParOf" srcId="{CFE0E388-3CD6-40F8-B605-5B464D20B2E5}" destId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{BD0C2D58-FF0A-4326-A798-5C83930D97A6}" type="presParOf" srcId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" destId="{0F8A7C2B-1759-4FB3-8042-677439E48219}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{3BA73BE5-A34E-495D-8F83-514C7309D67E}" type="presParOf" srcId="{0F8A7C2B-1759-4FB3-8042-677439E48219}" destId="{F5B18884-E498-499B-92AD-14DA40157B0A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{0F9838D9-97F0-4AB4-8D17-AFB5A070FB9D}" type="presParOf" srcId="{0F8A7C2B-1759-4FB3-8042-677439E48219}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{3E07F819-BDC9-41FE-831F-1204B51E0B42}" type="presParOf" srcId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" destId="{323A9B1A-E968-47F7-BED6-41A759F568C3}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6730EDD0-4BD8-4D84-9E15-0805530D32D5}" type="presParOf" srcId="{E13984DD-BA89-4F59-8902-36673B32B7C7}" destId="{34F96038-D67A-46A4-B7CA-55B5FE28E7CF}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{279C6EBB-133C-4E6A-8A5D-81C9DA0FA25F}" type="presParOf" srcId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" destId="{25801B8D-95D6-48CD-93F1-3025ED251512}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{C1B2E15B-339B-49EF-BF3B-027ACC0E59DA}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="8" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{508C222C-984B-43CB-AEE8-D3B8BA1C3E66}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{023D105C-727F-4B80-853C-64AB2A0F3749}" srcOrd="9" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{915D5309-38ED-48C0-9F65-59EF6BEB30C3}" type="presParOf" srcId="{023D105C-727F-4B80-853C-64AB2A0F3749}" destId="{8BC333C7-7439-44E7-B907-DB6755839F28}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2C79241E-735E-4DA4-B51F-797C25B01C41}" type="presParOf" srcId="{8BC333C7-7439-44E7-B907-DB6755839F28}" destId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6675AAF4-9A5F-429F-8D4D-CD462EB774C4}" type="presParOf" srcId="{8BC333C7-7439-44E7-B907-DB6755839F28}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{8CD847A0-44A6-422B-AD46-3129421629D7}" type="presParOf" srcId="{023D105C-727F-4B80-853C-64AB2A0F3749}" destId="{25BB545E-6C6F-4D7E-AC44-1F23E3318EF9}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{BE5D7FE6-3703-4638-80C6-FDE4432FA392}" type="presParOf" srcId="{023D105C-727F-4B80-853C-64AB2A0F3749}" destId="{E63BC231-8990-4828-933B-663A84A923E7}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{8B2C2F6E-90CB-40D2-8FBB-C8C260D19967}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="10" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{EC5AB199-C5BD-4E14-BF89-B01C1C6D7ABC}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{14920BCF-0F77-45F3-AF09-5773FB403370}" srcOrd="11" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{8210C6DF-57B2-4AEA-A29E-B043976803A5}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{951A5EBE-973F-49D2-AEE8-E9C1FD21E621}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9E6C5EE5-C097-48B9-9F17-93CA37EEB53D}" type="presParOf" srcId="{951A5EBE-973F-49D2-AEE8-E9C1FD21E621}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F4F38111-0959-4E30-8E76-B27D793DFD08}" type="presParOf" srcId="{951A5EBE-973F-49D2-AEE8-E9C1FD21E621}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{A662CC20-B897-4C23-BE86-052F51FE0961}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{5154CB22-61FB-414C-948D-B5CAB376CD6A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9938CBB7-1955-4A14-9738-70EC3065762F}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{E0CF165D-444F-4D0C-9894-0CEE601662E0}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{AF9273E8-AF53-4499-B8EE-B157657049B7}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="12" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{AEA0668E-5882-411E-A90E-9A18917A58B1}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" srcOrd="13" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E22B93FF-C5B5-40D0-9D8C-30BF0BBC24DC}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{65890E10-58E8-4BB6-AC06-53B5F5902D6D}" type="presParOf" srcId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" destId="{0FAB1775-08F8-482E-A204-647B49CA8593}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{21E81E96-CA96-4354-BA05-52A08BD70467}" type="presParOf" srcId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{A1551817-5CA6-4336-800C-150B1652172E}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{4AEBA50B-F3AB-455F-808A-6D8D6F6C8FC7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{DA3B8371-91A3-4863-94CB-876FC2B8007A}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{47D9F871-9894-4842-A60A-C9A1F58C3CB5}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{403888BF-165D-4DF9-99BD-77EA280BF47C}" type="presParOf" srcId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" destId="{4ACAA18A-FBAA-4144-A54E-57F8DC1C473C}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
   </dgm:cxnLst>
   <dgm:bg/>
@@ -2196,8 +2490,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3389976" y="2054922"/>
-          <a:ext cx="247913" cy="1599044"/>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="1667208"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2211,13 +2505,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="1599044"/>
+                <a:pt x="96930" y="1667208"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="1599044"/>
+                <a:pt x="193861" y="1667208"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2257,8 +2551,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3389976" y="2054922"/>
-          <a:ext cx="247913" cy="1066029"/>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="1250406"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2272,13 +2566,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="1066029"/>
+                <a:pt x="96930" y="1250406"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="1066029"/>
+                <a:pt x="193861" y="1250406"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2318,8 +2612,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3389976" y="2054922"/>
-          <a:ext cx="247913" cy="533014"/>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="833604"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2333,13 +2627,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="533014"/>
+                <a:pt x="96930" y="833604"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="533014"/>
+                <a:pt x="193861" y="833604"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2379,8 +2673,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4877459" y="2054922"/>
-          <a:ext cx="247913" cy="266507"/>
+          <a:off x="4742328" y="2442671"/>
+          <a:ext cx="193861" cy="208401"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2394,13 +2688,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="266507"/>
+                <a:pt x="96930" y="208401"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="266507"/>
+                <a:pt x="193861" y="208401"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2440,8 +2734,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4877459" y="1788415"/>
-          <a:ext cx="247913" cy="266507"/>
+          <a:off x="4742328" y="2234270"/>
+          <a:ext cx="193861" cy="208401"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2452,16 +2746,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="266507"/>
+                <a:pt x="0" y="208401"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="266507"/>
+                <a:pt x="96930" y="208401"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="0"/>
+                <a:pt x="193861" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2501,8 +2795,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3389976" y="2009202"/>
-          <a:ext cx="247913" cy="91440"/>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="416802"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2513,10 +2807,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="45720"/>
+                <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="247913" y="45720"/>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="416802"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="416802"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2556,8 +2856,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3389976" y="1521907"/>
-          <a:ext cx="247913" cy="533014"/>
+          <a:off x="3579160" y="1817468"/>
+          <a:ext cx="193861" cy="208401"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2568,16 +2868,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="533014"/>
+                <a:pt x="0" y="208401"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="533014"/>
+                <a:pt x="96930" y="208401"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="0"/>
+                <a:pt x="193861" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2610,15 +2910,15 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
     </dsp:sp>
-    <dsp:sp modelId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}">
+    <dsp:sp modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3389976" y="988892"/>
-          <a:ext cx="247913" cy="1066029"/>
+          <a:off x="4742328" y="1400666"/>
+          <a:ext cx="193861" cy="416802"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2629,16 +2929,193 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="1066029"/>
+                <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="1066029"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="416802"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="0"/>
+                <a:pt x="193861" y="416802"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{224BDC60-7934-422F-B29C-84F028B56716}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="1354946"/>
+          <a:ext cx="193861" cy="91440"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="45720"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="193861" y="45720"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="983864"/>
+          <a:ext cx="193861" cy="416802"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="416802"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="416802"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="1400666"/>
+          <a:ext cx="193861" cy="625203"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="625203"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="625203"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2678,8 +3155,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4877459" y="455877"/>
-          <a:ext cx="247913" cy="266507"/>
+          <a:off x="4742328" y="358661"/>
+          <a:ext cx="193861" cy="208401"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2693,13 +3170,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="266507"/>
+                <a:pt x="96930" y="208401"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="266507"/>
+                <a:pt x="193861" y="208401"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2739,8 +3216,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4877459" y="189370"/>
-          <a:ext cx="247913" cy="266507"/>
+          <a:off x="4742328" y="150260"/>
+          <a:ext cx="193861" cy="208401"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2751,16 +3228,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="266507"/>
+                <a:pt x="0" y="208401"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="266507"/>
+                <a:pt x="96930" y="208401"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="0"/>
+                <a:pt x="193861" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2800,8 +3277,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3389976" y="455877"/>
-          <a:ext cx="247913" cy="1599044"/>
+          <a:off x="3579160" y="358661"/>
+          <a:ext cx="193861" cy="1667208"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2812,16 +3289,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="1599044"/>
+                <a:pt x="0" y="1667208"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="123956" y="1599044"/>
+                <a:pt x="96930" y="1667208"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="123956" y="0"/>
+                <a:pt x="96930" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="247913" y="0"/>
+                <a:pt x="193861" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2861,8 +3338,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2150406" y="1865888"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="2609852" y="1878050"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2903,12 +3380,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2920,15 +3397,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
             <a:t>(index)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2150406" y="1865888"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="2609852" y="1878050"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}">
@@ -2938,8 +3415,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3637890" y="266843"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="3773021" y="210841"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2980,12 +3457,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -2997,15 +3474,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
             <a:t>(survey)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3637890" y="266843"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="3773021" y="210841"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}">
@@ -3015,8 +3492,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5125373" y="335"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="4936189" y="2440"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3057,12 +3534,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3074,15 +3551,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
             <a:t>(vote)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5125373" y="335"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="4936189" y="2440"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}">
@@ -3092,8 +3569,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="5125373" y="533350"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="4936189" y="419242"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3134,12 +3611,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3151,15 +3628,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
             <a:t>view</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="5125373" y="533350"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="4936189" y="419242"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}">
@@ -3169,8 +3646,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3637890" y="799858"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="3773021" y="1252847"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3211,12 +3688,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3228,26 +3705,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>create</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>make</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3637890" y="799858"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="3773021" y="1252847"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
+    <dsp:sp modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3637890" y="1332873"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="4936189" y="836045"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3288,12 +3765,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3305,227 +3782,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>my(page)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>check</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3637890" y="1332873"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="4936189" y="836045"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
+    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3637890" y="1865888"/>
-          <a:ext cx="1239569" cy="378068"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>auth</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3637890" y="1865888"/>
-        <a:ext cx="1239569" cy="378068"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5125373" y="1599380"/>
-          <a:ext cx="1239569" cy="378068"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>(login)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="5125373" y="1599380"/>
-        <a:ext cx="1239569" cy="378068"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5125373" y="2132395"/>
-          <a:ext cx="1239569" cy="378068"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>logout</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="5125373" y="2132395"/>
-        <a:ext cx="1239569" cy="378068"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3637890" y="2398903"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="4936189" y="1252847"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3566,12 +3842,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3583,26 +3859,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>tag</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3637890" y="2398903"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="4936189" y="1252847"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
+    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3637890" y="2931918"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="4936189" y="1669649"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3643,12 +3919,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3660,26 +3936,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>user</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>end</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3637890" y="2931918"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="4936189" y="1669649"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}">
+    <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3637890" y="3464933"/>
-          <a:ext cx="1239569" cy="378068"/>
+          <a:off x="3773021" y="1669649"/>
+          <a:ext cx="969307" cy="295638"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3720,12 +3996,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="15240" tIns="15240" rIns="15240" bIns="15240" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="1066800">
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3737,15 +4013,447 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="2400" kern="1200"/>
-            <a:t>favorite</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="2400" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>my(page)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3637890" y="3464933"/>
-        <a:ext cx="1239569" cy="378068"/>
+        <a:off x="3773021" y="1669649"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="2294852"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>auth</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="2294852"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="2086451"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>(login)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="2086451"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="2503253"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>logout</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="2503253"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="2711654"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>tag</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="2711654"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="3128456"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>user</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="3128456"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="3545258"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>favorite</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="3545258"/>
+        <a:ext cx="969307" cy="295638"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -12333,7 +13041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
@@ -12401,8 +13109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="N14:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
update view add survey panel
</commit_message>
<xml_diff>
--- a/view_plan.xlsx
+++ b/view_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355" activeTab="5"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="all_page_view" sheetId="6" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="make" sheetId="4" r:id="rId5"/>
     <sheet name="make_end" sheetId="7" r:id="rId6"/>
     <sheet name="mypage" sheetId="3" r:id="rId7"/>
+    <sheet name="survey_panel" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -1745,6 +1746,13 @@
     <dgm:pt modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" type="pres">
       <dgm:prSet presAssocID="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="7"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{83391BB5-AFDB-487B-8E65-A8933F5D40C0}" type="pres">
       <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="hierRoot2" presStyleCnt="0">
@@ -1795,6 +1803,13 @@
     <dgm:pt modelId="{224BDC60-7934-422F-B29C-84F028B56716}" type="pres">
       <dgm:prSet presAssocID="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="7"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{02B42FDE-E435-4D7F-BCA4-7B0F81D6BEE7}" type="pres">
       <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="hierRoot2" presStyleCnt="0">
@@ -1845,6 +1860,13 @@
     <dgm:pt modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" type="pres">
       <dgm:prSet presAssocID="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="7"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{1CF3CCC9-8575-45C6-8D49-050F1EF2260B}" type="pres">
       <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="hierRoot2" presStyleCnt="0">
@@ -2301,66 +2323,66 @@
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
+    <dgm:cxn modelId="{7B55AD7D-CC95-45FE-BCFE-7B483051B4CB}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{33CBFE4F-047C-4EDF-8FBC-62953BACFD7B}" type="presOf" srcId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" destId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{215983E4-081D-4467-A756-55FEF443A562}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D823C5EF-1423-4863-AAC0-3CCB22E52AE5}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" srcOrd="0" destOrd="0" parTransId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" sibTransId="{EA4D083E-0312-47CC-8039-9496D55CDBDC}"/>
+    <dgm:cxn modelId="{0B25676A-30F3-4EC1-A0B7-586CBD08E376}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{28369DE3-437A-4135-B55E-48F1D6296DC6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{559ADFF3-0478-496C-AFD5-D9545B790EC4}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{FA5FD46B-9D83-45A4-9344-56D6066107F5}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B9E26008-760E-4F53-A157-28E1F48ABE00}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" srcOrd="0" destOrd="0" parTransId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" sibTransId="{0F0D26FC-9E72-450A-A689-3301417EC882}"/>
+    <dgm:cxn modelId="{EED1F78C-85BA-4908-9EDB-040048925EE2}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" srcOrd="0" destOrd="0" parTransId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" sibTransId="{D18382C1-3316-401F-B9F7-5740273EBE35}"/>
+    <dgm:cxn modelId="{442C35E7-9219-42B1-8589-CA6B5AFD7FD1}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" srcOrd="5" destOrd="0" parTransId="{16684A72-88D1-4068-9742-A287A1AF7991}" sibTransId="{E1FF0606-7FA7-4C21-8E5B-4C259D042C61}"/>
+    <dgm:cxn modelId="{814C55A4-746A-46AC-B71C-48916393BAC3}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{F5B18884-E498-499B-92AD-14DA40157B0A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E77DC00F-1DBC-4305-A75A-CA0AF88B6519}" type="presOf" srcId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" destId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7AC678BE-C1B9-4C2C-BBA5-63C6027EC514}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2415E457-D5E9-475F-B3CE-4993C41B9B2A}" type="presOf" srcId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" destId="{9451D74F-6692-4FF1-A580-5574CD4401DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F5EBD142-F152-4BD8-AE52-4066178EEE6D}" type="presOf" srcId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{DE057FFD-529A-4E2E-B498-BC5F7742815B}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{078BFD8E-7E7A-44CB-8C2A-862AA6B7EF64}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{1B7EE4ED-C343-4DBF-8592-DAF824F32B4F}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{5AD42C2B-3B72-4332-8CB0-CB02483CBB7A}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{0A3BCE5E-23D3-4914-A0DE-4D82B34706DE}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" srcOrd="0" destOrd="0" parTransId="{CCD73AB5-5FAC-49DE-B051-A16352DE18B0}" sibTransId="{90EBE641-EF69-4D14-98EF-9FFC06AA100B}"/>
+    <dgm:cxn modelId="{35A1554D-6075-49F2-94F5-D41A56B41CB3}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{BEE184DB-6F27-4D7A-9C18-98A0A01EDA70}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F30AFEB2-A830-4035-BA71-EB491C42489C}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" srcOrd="0" destOrd="0" parTransId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" sibTransId="{E8DF5D1F-4EAF-4749-95FB-4BF5DDF36D94}"/>
+    <dgm:cxn modelId="{97FB1D32-8AB3-45A8-8D63-292929166F76}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" srcOrd="1" destOrd="0" parTransId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" sibTransId="{2AD778EF-0F85-4883-B9FB-FEB9810673D5}"/>
+    <dgm:cxn modelId="{2135CB57-A821-4A45-B869-6D0CF021FCED}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" srcOrd="4" destOrd="0" parTransId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" sibTransId="{49B5EA05-D380-4B41-9D7A-E2087005D6BD}"/>
+    <dgm:cxn modelId="{815260D8-FCB5-45E3-8AFB-F460679B2CDE}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{92107E38-7630-470C-9791-C19A37DEC9FA}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{B2A681BD-5EE0-45B6-B4F9-016D77485296}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9F01A4C8-FCDC-41BC-898B-747FEC5B6389}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1117B828-D277-43FA-B244-6FF95B68193E}" type="presOf" srcId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{38BB76FF-0FA4-4F6D-A1F3-00F631A74DDB}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" srcOrd="3" destOrd="0" parTransId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" sibTransId="{DA3E9CE7-349A-4E9E-BD8A-D3E3EE2D990C}"/>
+    <dgm:cxn modelId="{D01C7126-32B6-4DB4-833B-0C12061AE485}" type="presOf" srcId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" destId="{224BDC60-7934-422F-B29C-84F028B56716}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{752DC3CA-1459-43DF-8D17-59075C9B7B68}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="1" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
+    <dgm:cxn modelId="{32C55363-4473-460E-A765-20AB775E2E35}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{DC212456-5040-4495-9F5E-3AA3C3560C20}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FE9E3000-93A4-4B79-A18F-D60B82D46552}" type="presOf" srcId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{6B143136-E6DE-46E8-9AD5-1977D53BF989}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{0FAB1775-08F8-482E-A204-647B49CA8593}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{320201D6-8AE1-4176-9635-D81197B9E8AD}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{56247623-20AE-45E9-A8C5-000B0DE85F7F}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{82F277AB-87C7-433B-862F-87C13847027E}" srcOrd="1" destOrd="0" parTransId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" sibTransId="{8C3C1181-DF4B-4EE3-9ED3-562C8BC3A0A0}"/>
+    <dgm:cxn modelId="{E929C590-2797-4F5F-A36A-48FC41BCAC3F}" type="presOf" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FC7B3FFE-23C2-480C-9156-521BA5E4ED21}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{B7442801-F217-4912-AE49-8224D444B7AE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{0A3BCE5E-23D3-4914-A0DE-4D82B34706DE}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" srcOrd="0" destOrd="0" parTransId="{CCD73AB5-5FAC-49DE-B051-A16352DE18B0}" sibTransId="{90EBE641-EF69-4D14-98EF-9FFC06AA100B}"/>
+    <dgm:cxn modelId="{D0A170FC-0AB5-4AEF-91B1-1D414CCEFE41}" type="presOf" srcId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6DB29CA3-84E3-4AE3-B269-0E4E9A2370AB}" type="presOf" srcId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" destId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{3F8AEC38-DCAC-422E-BBE1-60F8D32065DD}" type="presOf" srcId="{16684A72-88D1-4068-9742-A287A1AF7991}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{5AD42C2B-3B72-4332-8CB0-CB02483CBB7A}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{AD187AFA-F1B3-417B-A18B-1DA461641B00}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{BB4B00DC-A343-4429-9992-C97EBA76F0AA}" type="presOf" srcId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{47E9E0D7-561B-4062-99B9-8E5422CA1060}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{1103E670-28FF-4AB2-9FAA-8999DB660777}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" srcOrd="1" destOrd="0" parTransId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" sibTransId="{0F39B1C9-85F1-4DD3-8B99-1EDD809C502C}"/>
-    <dgm:cxn modelId="{6DB29CA3-84E3-4AE3-B269-0E4E9A2370AB}" type="presOf" srcId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" destId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{63A697A5-BE9C-4F91-A92C-3506C14F0A22}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D8ED3677-8BE0-47AD-826F-58E9D454D3D0}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1C6CD132-06CD-4B2C-8DDD-553AE71D597C}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B0C83AA9-272C-4A44-AC90-24DE78B5CC49}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{83B3D6F2-C63A-4120-828B-5A15440C2D24}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{404FFDC8-1807-40B1-88B3-D52B6630D710}" type="presOf" srcId="{CEED879D-C918-490C-A079-5102097205A7}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" srcOrd="2" destOrd="0" parTransId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" sibTransId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}"/>
+    <dgm:cxn modelId="{FA5FD46B-9D83-45A4-9344-56D6066107F5}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7BDC27E4-38E1-44C6-9275-7D0DAB391DBF}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" srcOrd="6" destOrd="0" parTransId="{CEED879D-C918-490C-A079-5102097205A7}" sibTransId="{96D318EA-92A6-4D06-8BD0-F3437FB33BA9}"/>
+    <dgm:cxn modelId="{38DBDA98-E1B6-4DF0-B945-0EC585B5EFB9}" type="presOf" srcId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" destId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{71DBFE96-B81B-465F-9F92-6E34F83D6304}" type="presOf" srcId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E1971364-B9C9-4F2D-8D2C-1C3FFC969523}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" srcOrd="2" destOrd="0" parTransId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" sibTransId="{12ED1614-9395-4694-B66E-BE7517C9B3C3}"/>
     <dgm:cxn modelId="{41EA2324-B53B-4930-BACB-AFDEA8715A7A}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{215983E4-081D-4467-A756-55FEF443A562}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{815260D8-FCB5-45E3-8AFB-F460679B2CDE}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{63A697A5-BE9C-4F91-A92C-3506C14F0A22}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{2415E457-D5E9-475F-B3CE-4993C41B9B2A}" type="presOf" srcId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" destId="{9451D74F-6692-4FF1-A580-5574CD4401DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{32C55363-4473-460E-A765-20AB775E2E35}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{EED1F78C-85BA-4908-9EDB-040048925EE2}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" srcOrd="0" destOrd="0" parTransId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" sibTransId="{D18382C1-3316-401F-B9F7-5740273EBE35}"/>
-    <dgm:cxn modelId="{752DC3CA-1459-43DF-8D17-59075C9B7B68}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{83B3D6F2-C63A-4120-828B-5A15440C2D24}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D01C7126-32B6-4DB4-833B-0C12061AE485}" type="presOf" srcId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" destId="{224BDC60-7934-422F-B29C-84F028B56716}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{FC7B3FFE-23C2-480C-9156-521BA5E4ED21}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{B7442801-F217-4912-AE49-8224D444B7AE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{47E9E0D7-561B-4062-99B9-8E5422CA1060}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{404FFDC8-1807-40B1-88B3-D52B6630D710}" type="presOf" srcId="{CEED879D-C918-490C-A079-5102097205A7}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{FE9E3000-93A4-4B79-A18F-D60B82D46552}" type="presOf" srcId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{BEE184DB-6F27-4D7A-9C18-98A0A01EDA70}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{7BDC27E4-38E1-44C6-9275-7D0DAB391DBF}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D8ED3677-8BE0-47AD-826F-58E9D454D3D0}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" srcOrd="2" destOrd="0" parTransId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" sibTransId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}"/>
-    <dgm:cxn modelId="{33CBFE4F-047C-4EDF-8FBC-62953BACFD7B}" type="presOf" srcId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" destId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{7AC678BE-C1B9-4C2C-BBA5-63C6027EC514}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{35A1554D-6075-49F2-94F5-D41A56B41CB3}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{DC212456-5040-4495-9F5E-3AA3C3560C20}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{B9E26008-760E-4F53-A157-28E1F48ABE00}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" srcOrd="0" destOrd="0" parTransId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" sibTransId="{0F0D26FC-9E72-450A-A689-3301417EC882}"/>
-    <dgm:cxn modelId="{DE057FFD-529A-4E2E-B498-BC5F7742815B}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{078BFD8E-7E7A-44CB-8C2A-862AA6B7EF64}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D823C5EF-1423-4863-AAC0-3CCB22E52AE5}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" srcOrd="0" destOrd="0" parTransId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" sibTransId="{EA4D083E-0312-47CC-8039-9496D55CDBDC}"/>
-    <dgm:cxn modelId="{E929C590-2797-4F5F-A36A-48FC41BCAC3F}" type="presOf" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{3F8AEC38-DCAC-422E-BBE1-60F8D32065DD}" type="presOf" srcId="{16684A72-88D1-4068-9742-A287A1AF7991}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{97FB1D32-8AB3-45A8-8D63-292929166F76}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" srcOrd="1" destOrd="0" parTransId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" sibTransId="{2AD778EF-0F85-4883-B9FB-FEB9810673D5}"/>
-    <dgm:cxn modelId="{38BB76FF-0FA4-4F6D-A1F3-00F631A74DDB}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" srcOrd="3" destOrd="0" parTransId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" sibTransId="{DA3E9CE7-349A-4E9E-BD8A-D3E3EE2D990C}"/>
-    <dgm:cxn modelId="{AD187AFA-F1B3-417B-A18B-1DA461641B00}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{2135CB57-A821-4A45-B869-6D0CF021FCED}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" srcOrd="4" destOrd="0" parTransId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" sibTransId="{49B5EA05-D380-4B41-9D7A-E2087005D6BD}"/>
-    <dgm:cxn modelId="{BB4B00DC-A343-4429-9992-C97EBA76F0AA}" type="presOf" srcId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E1971364-B9C9-4F2D-8D2C-1C3FFC969523}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" srcOrd="2" destOrd="0" parTransId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" sibTransId="{12ED1614-9395-4694-B66E-BE7517C9B3C3}"/>
-    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="1" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
-    <dgm:cxn modelId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" srcOrd="6" destOrd="0" parTransId="{CEED879D-C918-490C-A079-5102097205A7}" sibTransId="{96D318EA-92A6-4D06-8BD0-F3437FB33BA9}"/>
-    <dgm:cxn modelId="{F30AFEB2-A830-4035-BA71-EB491C42489C}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" srcOrd="0" destOrd="0" parTransId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" sibTransId="{E8DF5D1F-4EAF-4749-95FB-4BF5DDF36D94}"/>
-    <dgm:cxn modelId="{0B25676A-30F3-4EC1-A0B7-586CBD08E376}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{28369DE3-437A-4135-B55E-48F1D6296DC6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{442C35E7-9219-42B1-8589-CA6B5AFD7FD1}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" srcOrd="5" destOrd="0" parTransId="{16684A72-88D1-4068-9742-A287A1AF7991}" sibTransId="{E1FF0606-7FA7-4C21-8E5B-4C259D042C61}"/>
-    <dgm:cxn modelId="{71DBFE96-B81B-465F-9F92-6E34F83D6304}" type="presOf" srcId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{38DBDA98-E1B6-4DF0-B945-0EC585B5EFB9}" type="presOf" srcId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" destId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E77DC00F-1DBC-4305-A75A-CA0AF88B6519}" type="presOf" srcId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" destId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{9F01A4C8-FCDC-41BC-898B-747FEC5B6389}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{B0C83AA9-272C-4A44-AC90-24DE78B5CC49}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{1117B828-D277-43FA-B244-6FF95B68193E}" type="presOf" srcId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F5EBD142-F152-4BD8-AE52-4066178EEE6D}" type="presOf" srcId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{56247623-20AE-45E9-A8C5-000B0DE85F7F}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{82F277AB-87C7-433B-862F-87C13847027E}" srcOrd="1" destOrd="0" parTransId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" sibTransId="{8C3C1181-DF4B-4EE3-9ED3-562C8BC3A0A0}"/>
-    <dgm:cxn modelId="{814C55A4-746A-46AC-B71C-48916393BAC3}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{F5B18884-E498-499B-92AD-14DA40157B0A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D0A170FC-0AB5-4AEF-91B1-1D414CCEFE41}" type="presOf" srcId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{92107E38-7630-470C-9791-C19A37DEC9FA}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{B2A681BD-5EE0-45B6-B4F9-016D77485296}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{1C6CD132-06CD-4B2C-8DDD-553AE71D597C}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{7B55AD7D-CC95-45FE-BCFE-7B483051B4CB}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{2D7F7C22-ADD5-4E45-A535-C589EB253F20}" type="presParOf" srcId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" destId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{C9F10509-5022-4B9B-A341-CC3365CCCF88}" type="presParOf" srcId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" destId="{87B98112-BB49-47E9-92F1-82F9448578BD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{CDA112DB-C227-483A-BA50-1640272F1F9E}" type="presParOf" srcId="{87B98112-BB49-47E9-92F1-82F9448578BD}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2484,1979 +2506,6 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
-    <dsp:sp modelId="{FE068172-564A-4253-AF89-D2BDB64E74DA}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="1667208"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="1667208"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="1667208"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{400A970B-01E2-495E-9ECB-7EADDBB33666}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="1250406"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="1250406"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="1250406"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="833604"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="833604"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="833604"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{94834600-2A81-4D2E-BA8C-D171F42E9531}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4742328" y="2442671"/>
-          <a:ext cx="193861" cy="208401"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="208401"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="208401"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4742328" y="2234270"/>
-          <a:ext cx="193861" cy="208401"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="208401"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="208401"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{E0568980-BD26-44B0-99C5-2B5582E6C423}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="416802"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="416802"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="416802"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3579160" y="1817468"/>
-          <a:ext cx="193861" cy="208401"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="208401"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="208401"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4742328" y="1400666"/>
-          <a:ext cx="193861" cy="416802"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="416802"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="416802"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{224BDC60-7934-422F-B29C-84F028B56716}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4742328" y="1354946"/>
-          <a:ext cx="193861" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="193861" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4742328" y="983864"/>
-          <a:ext cx="193861" cy="416802"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="416802"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="416802"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3579160" y="1400666"/>
-          <a:ext cx="193861" cy="625203"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="625203"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="625203"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4742328" y="358661"/>
-          <a:ext cx="193861" cy="208401"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="208401"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="208401"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4742328" y="150260"/>
-          <a:ext cx="193861" cy="208401"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="208401"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="208401"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{9451D74F-6692-4FF1-A580-5574CD4401DB}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3579160" y="358661"/>
-          <a:ext cx="193861" cy="1667208"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="1667208"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="96930" y="1667208"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2609852" y="1878050"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>(index)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2609852" y="1878050"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="210841"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>(survey)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="210841"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="2440"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>(vote)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="2440"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="419242"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>view</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="419242"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="1252847"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>make</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="1252847"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="836045"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>check</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="836045"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="1252847"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>regist</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="1252847"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="1669649"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>end</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="1669649"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="1669649"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>my(page)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="1669649"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="2294852"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>auth</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="2294852"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="2086451"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>(login)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="2086451"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="2503253"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>logout</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="2503253"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="2711654"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>tag</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="2711654"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="3128456"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>user</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="3128456"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="3545258"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>favorite</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="3545258"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
   </dsp:spTree>
 </dsp:drawing>
 </file>
@@ -12982,6 +11031,752 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2562225" y="923925"/>
+          <a:ext cx="8439150" cy="2981325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66676</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3419475" y="1095376"/>
+          <a:ext cx="7362825" cy="819149"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="3200"/>
+            <a:t>投票タイトル</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="3200"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>38102</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2733674" y="2438402"/>
+          <a:ext cx="1695451" cy="733424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>アイテム</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>533399</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47627</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4648199" y="2447927"/>
+          <a:ext cx="1695451" cy="733424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342899</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6515099" y="2486027"/>
+          <a:ext cx="1695451" cy="733424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>85727</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="正方形/長方形 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8381999" y="2486027"/>
+          <a:ext cx="1695451" cy="733424"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>161926</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="正方形/長方形 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2781300" y="3381374"/>
+          <a:ext cx="809626" cy="361951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>タグ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>409576</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="正方形/長方形 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3714750" y="3381374"/>
+          <a:ext cx="809626" cy="361951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>19051</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="正方形/長方形 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4695825" y="3381374"/>
+          <a:ext cx="809626" cy="361951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>247651</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5610225" y="3381374"/>
+          <a:ext cx="809626" cy="361951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438151</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="正方形/長方形 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6486525" y="3381374"/>
+          <a:ext cx="809626" cy="361951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>628651</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7362825" y="3381374"/>
+          <a:ext cx="809626" cy="361951"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="正方形/長方形 13"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2762249" y="1219200"/>
+          <a:ext cx="419101" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="3">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133352</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="正方形/長方形 14"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2733674" y="2019302"/>
+          <a:ext cx="7981951" cy="390523"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>詳細</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office ​​テーマ">
   <a:themeElements>
@@ -13317,7 +12112,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="AA31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -13366,8 +12161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -13382,11 +12177,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A4" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData/>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
create urlhelper update comp makeend module
</commit_message>
<xml_diff>
--- a/view_plan.xlsx
+++ b/view_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355"/>
   </bookViews>
   <sheets>
     <sheet name="all_page_view" sheetId="6" r:id="rId1"/>
@@ -2506,6 +2506,1979 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
+    <dsp:sp modelId="{FE068172-564A-4253-AF89-D2BDB64E74DA}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="1667208"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="1667208"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="1667208"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{400A970B-01E2-495E-9ECB-7EADDBB33666}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="1250406"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="1250406"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="1250406"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="833604"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="833604"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="833604"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{94834600-2A81-4D2E-BA8C-D171F42E9531}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="2442671"/>
+          <a:ext cx="193861" cy="208401"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="208401"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="208401"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="2234270"/>
+          <a:ext cx="193861" cy="208401"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="208401"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="208401"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{E0568980-BD26-44B0-99C5-2B5582E6C423}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="2025869"/>
+          <a:ext cx="193861" cy="416802"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="416802"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="416802"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="1817468"/>
+          <a:ext cx="193861" cy="208401"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="208401"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="208401"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="1400666"/>
+          <a:ext cx="193861" cy="416802"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="416802"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="416802"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{224BDC60-7934-422F-B29C-84F028B56716}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="1354946"/>
+          <a:ext cx="193861" cy="91440"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="45720"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="193861" y="45720"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="983864"/>
+          <a:ext cx="193861" cy="416802"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="416802"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="416802"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="1400666"/>
+          <a:ext cx="193861" cy="625203"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="625203"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="625203"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="358661"/>
+          <a:ext cx="193861" cy="208401"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="208401"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="208401"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4742328" y="150260"/>
+          <a:ext cx="193861" cy="208401"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="208401"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="208401"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{9451D74F-6692-4FF1-A580-5574CD4401DB}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3579160" y="358661"/>
+          <a:ext cx="193861" cy="1667208"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="1667208"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="96930" y="1667208"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="96930" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="193861" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2609852" y="1878050"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>(index)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2609852" y="1878050"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="210841"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>(survey)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="210841"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="2440"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>(vote)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="2440"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="419242"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>view</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="419242"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="1252847"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>make</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="1252847"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="836045"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>check</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="836045"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="1252847"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="1252847"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="1669649"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>end</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="1669649"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="1669649"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>my(page)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="1669649"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="2294852"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>auth</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="2294852"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="2086451"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>(login)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="2086451"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4936189" y="2503253"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>logout</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4936189" y="2503253"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="2711654"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>tag</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="2711654"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="3128456"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>user</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="3128456"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3773021" y="3545258"/>
+          <a:ext cx="969307" cy="295638"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:t>favorite</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3773021" y="3545258"/>
+        <a:ext cx="969307" cy="295638"/>
+      </dsp:txXfrm>
+    </dsp:sp>
   </dsp:spTree>
 </dsp:drawing>
 </file>
@@ -12066,7 +14039,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
@@ -12190,7 +14163,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update selectforms target hideframe
</commit_message>
<xml_diff>
--- a/view_plan.xlsx
+++ b/view_plan.xlsx
@@ -969,7 +969,22 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CCB51DA8-C62A-439F-B252-D6569840A52F}">
-      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1347,7 +1362,22 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{629E773C-EE7D-482A-94D1-6BB3211F734D}">
-      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1384,7 +1414,22 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9019F039-A6BB-4811-9BF3-881F48EB4453}">
-      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1421,7 +1466,22 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}">
-      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1447,6 +1507,58 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}" type="sibTrans" cxnId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" type="parTrans" cxnId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{457716A4-F71B-4FD3-8107-7455FE567B34}" type="sibTrans" cxnId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1573,7 +1685,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" type="pres">
-      <dgm:prSet presAssocID="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1596,7 +1708,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" type="pres">
-      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="7">
+      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="8">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1611,7 +1723,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" type="pres">
-      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1629,8 +1741,58 @@
       <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="hierChild5" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
+    <dgm:pt modelId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}" type="pres">
+      <dgm:prSet presAssocID="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="8"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2F50DF6C-A261-42AC-AE20-41E43651D22F}" type="pres">
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{AD7F183A-697D-41D3-958C-05CF2D020A5F}" type="pres">
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}" type="pres">
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="8">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CDDBF60B-A81F-49D1-8951-61E79769BB23}" type="pres">
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="8"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AAE90222-E6B3-4278-AA83-CEBF4F4938C9}" type="pres">
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{311C98BF-922E-47C2-8B10-62279EBED995}" type="pres">
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
     <dgm:pt modelId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" type="pres">
-      <dgm:prSet presAssocID="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1653,7 +1815,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" type="pres">
-      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="7">
+      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootText" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="8">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1668,7 +1830,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" type="pres">
-      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1744,7 +1906,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" type="pres">
-      <dgm:prSet presAssocID="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1767,7 +1929,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" type="pres">
-      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootText" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="7">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootText" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="8">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1782,7 +1944,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" type="pres">
-      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1801,7 +1963,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{224BDC60-7934-422F-B29C-84F028B56716}" type="pres">
-      <dgm:prSet presAssocID="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1824,7 +1986,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" type="pres">
-      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootText" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="7">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootText" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="8">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1839,7 +2001,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" type="pres">
-      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1858,7 +2020,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" type="pres">
-      <dgm:prSet presAssocID="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1881,7 +2043,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" type="pres">
-      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootText" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="7">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootText" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="8">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1896,7 +2058,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" type="pres">
-      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2029,7 +2191,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" type="pres">
-      <dgm:prSet presAssocID="{CC820015-08D8-4836-A31C-2D63FBA54C31}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{CC820015-08D8-4836-A31C-2D63FBA54C31}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2052,7 +2214,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" type="pres">
-      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootText" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="7">
+      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootText" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="8">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2067,7 +2229,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" type="pres">
-      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2086,7 +2248,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" type="pres">
-      <dgm:prSet presAssocID="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2109,7 +2271,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}" type="pres">
-      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootText" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="7">
+      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootText" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="8">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2124,7 +2286,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8D67E224-0EDF-448A-9790-7C530F95D644}" type="pres">
-      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="7"/>
+      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="8"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2337,7 +2499,9 @@
     <dgm:cxn modelId="{7AC678BE-C1B9-4C2C-BBA5-63C6027EC514}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{2415E457-D5E9-475F-B3CE-4993C41B9B2A}" type="presOf" srcId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" destId="{9451D74F-6692-4FF1-A580-5574CD4401DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{F5EBD142-F152-4BD8-AE52-4066178EEE6D}" type="presOf" srcId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1C8DA176-6832-4A0E-81F3-4837C501AC26}" type="presOf" srcId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" destId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{DE057FFD-529A-4E2E-B498-BC5F7742815B}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{078BFD8E-7E7A-44CB-8C2A-862AA6B7EF64}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" srcOrd="1" destOrd="0" parTransId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" sibTransId="{457716A4-F71B-4FD3-8107-7455FE567B34}"/>
     <dgm:cxn modelId="{1B7EE4ED-C343-4DBF-8592-DAF824F32B4F}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{35A1554D-6075-49F2-94F5-D41A56B41CB3}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{BEE184DB-6F27-4D7A-9C18-98A0A01EDA70}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2351,7 +2515,7 @@
     <dgm:cxn modelId="{38BB76FF-0FA4-4F6D-A1F3-00F631A74DDB}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" srcOrd="3" destOrd="0" parTransId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" sibTransId="{DA3E9CE7-349A-4E9E-BD8A-D3E3EE2D990C}"/>
     <dgm:cxn modelId="{D01C7126-32B6-4DB4-833B-0C12061AE485}" type="presOf" srcId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" destId="{224BDC60-7934-422F-B29C-84F028B56716}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{752DC3CA-1459-43DF-8D17-59075C9B7B68}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="1" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
+    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="2" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
     <dgm:cxn modelId="{32C55363-4473-460E-A765-20AB775E2E35}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{DC212456-5040-4495-9F5E-3AA3C3560C20}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{FE9E3000-93A4-4B79-A18F-D60B82D46552}" type="presOf" srcId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2361,6 +2525,7 @@
     <dgm:cxn modelId="{E929C590-2797-4F5F-A36A-48FC41BCAC3F}" type="presOf" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{FC7B3FFE-23C2-480C-9156-521BA5E4ED21}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{B7442801-F217-4912-AE49-8224D444B7AE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{0A3BCE5E-23D3-4914-A0DE-4D82B34706DE}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" srcOrd="0" destOrd="0" parTransId="{CCD73AB5-5FAC-49DE-B051-A16352DE18B0}" sibTransId="{90EBE641-EF69-4D14-98EF-9FFC06AA100B}"/>
+    <dgm:cxn modelId="{95DEC58E-CCCE-4EB2-8D93-F883B57FB55D}" type="presOf" srcId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" destId="{CDDBF60B-A81F-49D1-8951-61E79769BB23}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{D0A170FC-0AB5-4AEF-91B1-1D414CCEFE41}" type="presOf" srcId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{6DB29CA3-84E3-4AE3-B269-0E4E9A2370AB}" type="presOf" srcId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" destId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{3F8AEC38-DCAC-422E-BBE1-60F8D32065DD}" type="presOf" srcId="{16684A72-88D1-4068-9742-A287A1AF7991}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2378,6 +2543,7 @@
     <dgm:cxn modelId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" srcOrd="2" destOrd="0" parTransId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" sibTransId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}"/>
     <dgm:cxn modelId="{FA5FD46B-9D83-45A4-9344-56D6066107F5}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{7BDC27E4-38E1-44C6-9275-7D0DAB391DBF}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{C1D1B42F-A616-40D8-84DC-A1AD40C3E0D0}" type="presOf" srcId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" destId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" srcOrd="6" destOrd="0" parTransId="{CEED879D-C918-490C-A079-5102097205A7}" sibTransId="{96D318EA-92A6-4D06-8BD0-F3437FB33BA9}"/>
     <dgm:cxn modelId="{38DBDA98-E1B6-4DF0-B945-0EC585B5EFB9}" type="presOf" srcId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" destId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{71DBFE96-B81B-465F-9F92-6E34F83D6304}" type="presOf" srcId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2401,8 +2567,15 @@
     <dgm:cxn modelId="{A664672F-AD4B-4B51-A4FC-734910ECC8B4}" type="presParOf" srcId="{CB63B714-B6F1-4E7B-8271-E62459B70A39}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{C3FAC606-9364-4320-A393-6BE425236775}" type="presParOf" srcId="{EF9A0C57-0D97-4FB5-B4A2-65517B791C2A}" destId="{CA88BD6B-68FF-4A3C-B7A1-A0AD3B15386B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{3F423195-78E2-40C7-B913-3C63230572C1}" type="presParOf" srcId="{EF9A0C57-0D97-4FB5-B4A2-65517B791C2A}" destId="{F2365550-9B51-4822-87D7-B8D09D6E375D}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F0FC7B76-FC04-462B-8FE1-EFF1FCB4D647}" type="presParOf" srcId="{79363F0A-16EA-4910-AD4E-4212F035E71A}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{1330495F-2E03-49C3-BCBF-027168158904}" type="presParOf" srcId="{79363F0A-16EA-4910-AD4E-4212F035E71A}" destId="{CC129583-6BE9-4C44-BBD9-A54B5DE203CE}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E048A696-3971-45C8-93A6-B5E0EFBE07F2}" type="presParOf" srcId="{79363F0A-16EA-4910-AD4E-4212F035E71A}" destId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B1B1AA4E-A298-4F86-9ED1-EC0589806474}" type="presParOf" srcId="{79363F0A-16EA-4910-AD4E-4212F035E71A}" destId="{2F50DF6C-A261-42AC-AE20-41E43651D22F}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9ACDF314-4ABA-4F7D-8C02-9AC2F0658ABF}" type="presParOf" srcId="{2F50DF6C-A261-42AC-AE20-41E43651D22F}" destId="{AD7F183A-697D-41D3-958C-05CF2D020A5F}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2EBE437A-D237-4E3C-AE76-50E3C5E3AC78}" type="presParOf" srcId="{AD7F183A-697D-41D3-958C-05CF2D020A5F}" destId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{177CE2C0-0988-4CCC-99F7-91628A09D8B1}" type="presParOf" srcId="{AD7F183A-697D-41D3-958C-05CF2D020A5F}" destId="{CDDBF60B-A81F-49D1-8951-61E79769BB23}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{DA0307B7-59FA-4E25-897D-FBED03B305DA}" type="presParOf" srcId="{2F50DF6C-A261-42AC-AE20-41E43651D22F}" destId="{AAE90222-E6B3-4278-AA83-CEBF4F4938C9}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{023E746C-2A0A-4608-927A-07746834C21E}" type="presParOf" srcId="{2F50DF6C-A261-42AC-AE20-41E43651D22F}" destId="{311C98BF-922E-47C2-8B10-62279EBED995}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F0FC7B76-FC04-462B-8FE1-EFF1FCB4D647}" type="presParOf" srcId="{79363F0A-16EA-4910-AD4E-4212F035E71A}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1330495F-2E03-49C3-BCBF-027168158904}" type="presParOf" srcId="{79363F0A-16EA-4910-AD4E-4212F035E71A}" destId="{CC129583-6BE9-4C44-BBD9-A54B5DE203CE}" srcOrd="5" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{8383640C-2884-41FD-8353-B8C9100AA71B}" type="presParOf" srcId="{CC129583-6BE9-4C44-BBD9-A54B5DE203CE}" destId="{E1C4C267-4392-4586-9669-FA34623D500E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{837F9CEF-43A0-4A65-91BD-B098D77150FF}" type="presParOf" srcId="{E1C4C267-4392-4586-9669-FA34623D500E}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{8EB7833E-EB35-4A76-91FD-DDED64F6738D}" type="presParOf" srcId="{E1C4C267-4392-4586-9669-FA34623D500E}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2513,8 +2686,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="1667208"/>
+          <a:off x="3645556" y="2109676"/>
+          <a:ext cx="174891" cy="1598067"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2528,13 +2701,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="1667208"/>
+                <a:pt x="87445" y="1598067"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="1667208"/>
+                <a:pt x="174891" y="1598067"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2574,8 +2747,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="1250406"/>
+          <a:off x="3645556" y="2109676"/>
+          <a:ext cx="174891" cy="1222051"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2589,13 +2762,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="1250406"/>
+                <a:pt x="87445" y="1222051"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="1250406"/>
+                <a:pt x="174891" y="1222051"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2635,8 +2808,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="833604"/>
+          <a:off x="3645556" y="2109676"/>
+          <a:ext cx="174891" cy="846035"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2650,13 +2823,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="833604"/>
+                <a:pt x="87445" y="846035"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="833604"/>
+                <a:pt x="174891" y="846035"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2696,8 +2869,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4742328" y="2442671"/>
-          <a:ext cx="193861" cy="208401"/>
+          <a:off x="4694902" y="2579696"/>
+          <a:ext cx="174891" cy="188007"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2711,13 +2884,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="208401"/>
+                <a:pt x="87445" y="188007"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="208401"/>
+                <a:pt x="174891" y="188007"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2757,8 +2930,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4742328" y="2234270"/>
-          <a:ext cx="193861" cy="208401"/>
+          <a:off x="4694902" y="2391688"/>
+          <a:ext cx="174891" cy="188007"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2769,16 +2942,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="208401"/>
+                <a:pt x="0" y="188007"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="208401"/>
+                <a:pt x="87445" y="188007"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="0"/>
+                <a:pt x="174891" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2818,8 +2991,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3579160" y="2025869"/>
-          <a:ext cx="193861" cy="416802"/>
+          <a:off x="3645556" y="2109676"/>
+          <a:ext cx="174891" cy="470019"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2833,13 +3006,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="416802"/>
+                <a:pt x="87445" y="470019"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="416802"/>
+                <a:pt x="174891" y="470019"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2879,8 +3052,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3579160" y="1817468"/>
-          <a:ext cx="193861" cy="208401"/>
+          <a:off x="3645556" y="2015672"/>
+          <a:ext cx="174891" cy="94003"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2891,16 +3064,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="208401"/>
+                <a:pt x="0" y="94003"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="208401"/>
+                <a:pt x="87445" y="94003"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="0"/>
+                <a:pt x="174891" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2940,8 +3113,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4742328" y="1400666"/>
-          <a:ext cx="193861" cy="416802"/>
+          <a:off x="4694902" y="1639657"/>
+          <a:ext cx="174891" cy="376015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2955,13 +3128,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="416802"/>
+                <a:pt x="87445" y="376015"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="416802"/>
+                <a:pt x="174891" y="376015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3001,8 +3174,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4742328" y="1354946"/>
-          <a:ext cx="193861" cy="91440"/>
+          <a:off x="4694902" y="1593937"/>
+          <a:ext cx="174891" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3016,7 +3189,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="193861" y="45720"/>
+                <a:pt x="174891" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3056,8 +3229,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4742328" y="983864"/>
-          <a:ext cx="193861" cy="416802"/>
+          <a:off x="4694902" y="1263641"/>
+          <a:ext cx="174891" cy="376015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3068,16 +3241,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="416802"/>
+                <a:pt x="0" y="376015"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="416802"/>
+                <a:pt x="87445" y="376015"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="0"/>
+                <a:pt x="174891" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3117,8 +3290,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3579160" y="1400666"/>
-          <a:ext cx="193861" cy="625203"/>
+          <a:off x="3645556" y="1639657"/>
+          <a:ext cx="174891" cy="470019"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3129,16 +3302,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="625203"/>
+                <a:pt x="0" y="470019"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="625203"/>
+                <a:pt x="87445" y="470019"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="0"/>
+                <a:pt x="174891" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3178,8 +3351,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4742328" y="358661"/>
-          <a:ext cx="193861" cy="208401"/>
+          <a:off x="4694902" y="511609"/>
+          <a:ext cx="174891" cy="376015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3193,13 +3366,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="208401"/>
+                <a:pt x="87445" y="376015"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="208401"/>
+                <a:pt x="174891" y="376015"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3232,15 +3405,15 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
     </dsp:sp>
-    <dsp:sp modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}">
+    <dsp:sp modelId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4742328" y="150260"/>
-          <a:ext cx="193861" cy="208401"/>
+          <a:off x="4694902" y="465889"/>
+          <a:ext cx="174891" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3251,16 +3424,10 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="208401"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="208401"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="96930" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="193861" y="0"/>
+                <a:pt x="174891" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3293,15 +3460,15 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
     </dsp:sp>
-    <dsp:sp modelId="{9451D74F-6692-4FF1-A580-5574CD4401DB}">
+    <dsp:sp modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3579160" y="358661"/>
-          <a:ext cx="193861" cy="1667208"/>
+          <a:off x="4694902" y="135593"/>
+          <a:ext cx="174891" cy="376015"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3312,16 +3479,77 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="1667208"/>
+                <a:pt x="0" y="376015"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="96930" y="1667208"/>
+                <a:pt x="87445" y="376015"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="96930" y="0"/>
+                <a:pt x="87445" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="193861" y="0"/>
+                <a:pt x="174891" y="0"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{9451D74F-6692-4FF1-A580-5574CD4401DB}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3645556" y="511609"/>
+          <a:ext cx="174891" cy="1598067"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="1598067"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="87445" y="1598067"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="87445" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="174891" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3361,8 +3589,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2609852" y="1878050"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="2771100" y="1976322"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3403,12 +3631,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3420,15 +3648,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
             <a:t>(index)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2609852" y="1878050"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="2771100" y="1976322"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}">
@@ -3438,8 +3666,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3773021" y="210841"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="3820447" y="378255"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3480,12 +3708,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3497,15 +3725,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
             <a:t>(survey)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3773021" y="210841"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="3820447" y="378255"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}">
@@ -3515,8 +3743,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4936189" y="2440"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="4869793" y="2239"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3557,12 +3785,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3574,15 +3802,82 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
             <a:t>(vote)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4936189" y="2440"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="4869793" y="2239"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4869793" y="378255"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4869793" y="378255"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}">
@@ -3592,8 +3887,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4936189" y="419242"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="4869793" y="754271"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3634,12 +3929,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3651,15 +3946,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
             <a:t>view</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4936189" y="419242"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="4869793" y="754271"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}">
@@ -3669,8 +3964,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3773021" y="1252847"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="3820447" y="1506302"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3711,12 +4006,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3728,15 +4023,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
             <a:t>make</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3773021" y="1252847"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="3820447" y="1506302"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}">
@@ -3746,8 +4041,564 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4936189" y="836045"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="4869793" y="1130286"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="accent5">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>check</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4869793" y="1130286"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4869793" y="1506302"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4869793" y="1506302"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4869793" y="1882318"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="accent5">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>end</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4869793" y="1882318"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3820447" y="1882318"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="accent5">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>my(page)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3820447" y="1882318"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3820447" y="2446342"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>auth</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3820447" y="2446342"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4869793" y="2258334"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>(login)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4869793" y="2258334"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4869793" y="2634350"/>
+          <a:ext cx="874455" cy="266708"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>logout</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4869793" y="2634350"/>
+        <a:ext cx="874455" cy="266708"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3820447" y="2822358"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3788,12 +4639,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3805,26 +4656,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>check</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>tag</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4936189" y="836045"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="3820447" y="2822358"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
+    <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4936189" y="1252847"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="3820447" y="3198373"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3865,12 +4716,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3882,26 +4733,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>regist</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>user</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4936189" y="1252847"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="3820447" y="3198373"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
+    <dsp:sp modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4936189" y="1669649"/>
-          <a:ext cx="969307" cy="295638"/>
+          <a:off x="3820447" y="3574389"/>
+          <a:ext cx="874455" cy="266708"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3942,12 +4793,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
+          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3959,524 +4810,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>end</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:t>favorite</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4936189" y="1669649"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="1669649"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>my(page)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="1669649"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="2294852"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>auth</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="2294852"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="2086451"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>(login)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="2086451"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4936189" y="2503253"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>logout</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4936189" y="2503253"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="2711654"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>tag</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="2711654"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="3128456"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>user</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="3128456"/>
-        <a:ext cx="969307" cy="295638"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3773021" y="3545258"/>
-          <a:ext cx="969307" cy="295638"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="12065" tIns="12065" rIns="12065" bIns="12065" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="844550">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1900" kern="1200"/>
-            <a:t>favorite</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1900" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3773021" y="3545258"/>
-        <a:ext cx="969307" cy="295638"/>
+        <a:off x="3820447" y="3574389"/>
+        <a:ext cx="874455" cy="266708"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -14039,7 +14381,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>

</xml_diff>

<commit_message>
update vote regist structure
</commit_message>
<xml_diff>
--- a/view_plan.xlsx
+++ b/view_plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355"/>
+    <workbookView xWindow="360" yWindow="30" windowWidth="5355" windowHeight="5355" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="all_page_view" sheetId="6" r:id="rId1"/>
@@ -932,7 +932,22 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{82F277AB-87C7-433B-862F-87C13847027E}">
-      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1021,7 +1036,22 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}">
-      <dgm:prSet phldrT="[テキスト]"/>
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent5"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent5"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1029,7 +1059,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>(vote)</a:t>
+            <a:t>vote</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
         </a:p>
@@ -1066,7 +1096,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>view</a:t>
+            <a:t>(view)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
         </a:p>
@@ -1324,8 +1354,23 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}">
-      <dgm:prSet phldrT="[テキスト]"/>
+    <dgm:pt modelId="{629E773C-EE7D-482A-94D1-6BB3211F734D}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1333,13 +1378,13 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>favorite</a:t>
+            <a:t>check</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{CEED879D-C918-490C-A079-5102097205A7}" type="parTrans" cxnId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}">
+    <dgm:pt modelId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" type="parTrans" cxnId="{EED1F78C-85BA-4908-9EDB-040048925EE2}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1350,7 +1395,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{96D318EA-92A6-4D06-8BD0-F3437FB33BA9}" type="sibTrans" cxnId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}">
+    <dgm:pt modelId="{D18382C1-3316-401F-B9F7-5740273EBE35}" type="sibTrans" cxnId="{EED1F78C-85BA-4908-9EDB-040048925EE2}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1361,7 +1406,429 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{629E773C-EE7D-482A-94D1-6BB3211F734D}">
+    <dgm:pt modelId="{9019F039-A6BB-4811-9BF3-881F48EB4453}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent3"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" type="parTrans" cxnId="{1103E670-28FF-4AB2-9FAA-8999DB660777}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0F39B1C9-85F1-4DD3-8B99-1EDD809C502C}" type="sibTrans" cxnId="{1103E670-28FF-4AB2-9FAA-8999DB660777}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>end</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" type="parTrans" cxnId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}" type="sibTrans" cxnId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" type="parTrans" cxnId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{457716A4-F71B-4FD3-8107-7455FE567B34}" type="sibTrans" cxnId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent6"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent6"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>hideTarget</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DA47D477-365A-4A74-AA96-5E5FEB632109}" type="parTrans" cxnId="{F81BCEF8-A95C-4677-921D-E34E2D2B1F37}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A56D162B-A8BF-4EE0-8EC5-7AA0A05D36B3}" type="sibTrans" cxnId="{F81BCEF8-A95C-4677-921D-E34E2D2B1F37}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>view</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D95BA311-15D4-4B2B-A05D-399473AB7692}" type="parTrans" cxnId="{C3D64037-6DDC-4D5F-B733-181307ADAF7C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{9915E53F-B0E6-44B6-B27E-B4A79CB3FBF7}" type="sibTrans" cxnId="{C3D64037-6DDC-4D5F-B733-181307ADAF7C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FA6FF089-541E-4496-A510-F6D4516B2FC8}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:fillRef>
+          <a:effectRef idx="1">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>userOnly</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C10D3E82-F9A1-462C-8FBA-5BD8E7806F8E}" type="parTrans" cxnId="{6EF22229-7E04-4838-8B5A-94EA53A1605C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{332702D0-9CA2-4E0B-A3FB-CA3318461BBD}" type="sibTrans" cxnId="{6EF22229-7E04-4838-8B5A-94EA53A1605C}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0FE1D759-A2B0-4446-9D87-B95385F80179}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="dk1"/>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="lt1"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="dk1"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>notView</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D6DCACAB-7D92-46B6-A2ED-8043909D48F3}" type="parTrans" cxnId="{F5416D48-C226-4944-A1DE-B8EE2E87FE6D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2A7A3AB8-E3AE-4CC4-8537-EDB1BCE1615B}" type="sibTrans" cxnId="{F5416D48-C226-4944-A1DE-B8EE2E87FE6D}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}">
+      <dgm:prSet phldrT="[テキスト]">
+        <dgm:style>
+          <a:lnRef idx="2">
+            <a:schemeClr val="accent3">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:lnRef>
+          <a:fillRef idx="1">
+            <a:schemeClr val="accent3"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:schemeClr val="accent3"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="lt1"/>
+          </a:fontRef>
+        </dgm:style>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
+            <a:t>notDirect</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B2F685BA-1AC9-4C10-A5F5-3E7531009405}" type="parTrans" cxnId="{8AC7FAB9-3355-47AA-A457-7136F862B206}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AFFCDD44-5217-4C68-A5FA-27C9C7E1E33C}" type="sibTrans" cxnId="{8AC7FAB9-3355-47AA-A457-7136F862B206}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A1986176-DBC3-405D-9BBF-0DA05F670219}">
       <dgm:prSet phldrT="[テキスト]">
         <dgm:style>
           <a:lnRef idx="1">
@@ -1385,13 +1852,13 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>check</a:t>
+            <a:t>fav(orite)</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" type="parTrans" cxnId="{EED1F78C-85BA-4908-9EDB-040048925EE2}">
+    <dgm:pt modelId="{5D3DE17C-EE5A-47BA-A905-F53770A94AE5}" type="parTrans" cxnId="{C5ADD361-091A-4ECF-8689-E6A3B7125DA0}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1402,163 +1869,7 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{D18382C1-3316-401F-B9F7-5740273EBE35}" type="sibTrans" cxnId="{EED1F78C-85BA-4908-9EDB-040048925EE2}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{9019F039-A6BB-4811-9BF3-881F48EB4453}">
-      <dgm:prSet phldrT="[テキスト]">
-        <dgm:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent5"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </dgm:style>
-      </dgm:prSet>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>regist</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" type="parTrans" cxnId="{1103E670-28FF-4AB2-9FAA-8999DB660777}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{0F39B1C9-85F1-4DD3-8B99-1EDD809C502C}" type="sibTrans" cxnId="{1103E670-28FF-4AB2-9FAA-8999DB660777}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}">
-      <dgm:prSet phldrT="[テキスト]">
-        <dgm:style>
-          <a:lnRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:lnRef>
-          <a:fillRef idx="2">
-            <a:schemeClr val="accent5"/>
-          </a:fillRef>
-          <a:effectRef idx="1">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </dgm:style>
-      </dgm:prSet>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>end</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" type="parTrans" cxnId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}" type="sibTrans" cxnId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}">
-      <dgm:prSet phldrT="[テキスト]">
-        <dgm:style>
-          <a:lnRef idx="2">
-            <a:schemeClr val="accent5"/>
-          </a:lnRef>
-          <a:fillRef idx="1">
-            <a:schemeClr val="lt1"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:schemeClr val="accent5"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </dgm:style>
-      </dgm:prSet>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP"/>
-            <a:t>regist</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" type="parTrans" cxnId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}">
-      <dgm:prSet/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{457716A4-F71B-4FD3-8107-7455FE567B34}" type="sibTrans" cxnId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}">
+    <dgm:pt modelId="{67DC55F0-7DFC-4F67-9A85-893F8218F853}" type="sibTrans" cxnId="{C5ADD361-091A-4ECF-8689-E6A3B7125DA0}">
       <dgm:prSet/>
       <dgm:spPr/>
       <dgm:t>
@@ -1602,7 +1913,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" type="pres">
-      <dgm:prSet presAssocID="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" presName="rootText1" presStyleLbl="node0" presStyleIdx="0" presStyleCnt="1">
+      <dgm:prSet presAssocID="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" presName="rootText1" presStyleLbl="node0" presStyleIdx="0" presStyleCnt="2">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1685,7 +1996,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" type="pres">
-      <dgm:prSet presAssocID="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="0" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1708,7 +2019,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" type="pres">
-      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="8">
+      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootText" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1723,7 +2034,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" type="pres">
-      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="0" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1742,8 +2053,15 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}" type="pres">
-      <dgm:prSet presAssocID="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="8"/>
-      <dgm:spPr/>
+      <dgm:prSet presAssocID="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="1" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{2F50DF6C-A261-42AC-AE20-41E43651D22F}" type="pres">
       <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="hierRoot2" presStyleCnt="0">
@@ -1758,7 +2076,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}" type="pres">
-      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="8">
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="rootText" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1773,7 +2091,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{CDDBF60B-A81F-49D1-8951-61E79769BB23}" type="pres">
-      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="1" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1792,7 +2110,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" type="pres">
-      <dgm:prSet presAssocID="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="2" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1815,7 +2133,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" type="pres">
-      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootText" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="8">
+      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootText" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1830,7 +2148,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" type="pres">
-      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="2" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1906,7 +2224,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" type="pres">
-      <dgm:prSet presAssocID="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="3" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1929,7 +2247,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" type="pres">
-      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootText" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="8">
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootText" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -1944,7 +2262,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" type="pres">
-      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{629E773C-EE7D-482A-94D1-6BB3211F734D}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="3" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1963,7 +2281,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{224BDC60-7934-422F-B29C-84F028B56716}" type="pres">
-      <dgm:prSet presAssocID="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="4" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -1986,7 +2304,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" type="pres">
-      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootText" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="8">
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootText" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2001,7 +2319,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" type="pres">
-      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{9019F039-A6BB-4811-9BF3-881F48EB4453}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="4" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2020,7 +2338,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" type="pres">
-      <dgm:prSet presAssocID="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="5" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2043,7 +2361,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" type="pres">
-      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootText" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="8">
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootText" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2058,7 +2376,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" type="pres">
-      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="5" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2133,6 +2451,56 @@
       <dgm:prSet presAssocID="{CCB51DA8-C62A-439F-B252-D6569840A52F}" presName="hierChild4" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
+    <dgm:pt modelId="{1A2B8F52-9746-463C-BC4A-04A1B691DD53}" type="pres">
+      <dgm:prSet presAssocID="{5D3DE17C-EE5A-47BA-A905-F53770A94AE5}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9F313496-2623-4AFE-A6FB-DA38AFC23721}" type="pres">
+      <dgm:prSet presAssocID="{A1986176-DBC3-405D-9BBF-0DA05F670219}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5D39ABD7-8940-4EB0-BD28-24328861EAC2}" type="pres">
+      <dgm:prSet presAssocID="{A1986176-DBC3-405D-9BBF-0DA05F670219}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B364BDD2-2468-482C-B4F5-1A0AB60AF7B9}" type="pres">
+      <dgm:prSet presAssocID="{A1986176-DBC3-405D-9BBF-0DA05F670219}" presName="rootText" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="10">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C375CBC5-A09F-4275-BCD3-62BA4354A038}" type="pres">
+      <dgm:prSet presAssocID="{A1986176-DBC3-405D-9BBF-0DA05F670219}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{EFA21C3A-FA62-4E09-874C-52C385FC8442}" type="pres">
+      <dgm:prSet presAssocID="{A1986176-DBC3-405D-9BBF-0DA05F670219}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{4966423A-AE1F-4EA5-97F1-80EF66672A6D}" type="pres">
+      <dgm:prSet presAssocID="{A1986176-DBC3-405D-9BBF-0DA05F670219}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
     <dgm:pt modelId="{0179D0B3-6350-4D61-9B67-663CD880CA02}" type="pres">
       <dgm:prSet presAssocID="{CCB51DA8-C62A-439F-B252-D6569840A52F}" presName="hierChild5" presStyleCnt="0"/>
       <dgm:spPr/>
@@ -2191,7 +2559,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" type="pres">
-      <dgm:prSet presAssocID="{CC820015-08D8-4836-A31C-2D63FBA54C31}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{CC820015-08D8-4836-A31C-2D63FBA54C31}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2214,7 +2582,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" type="pres">
-      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootText" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="8">
+      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootText" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2229,7 +2597,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" type="pres">
-      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="6" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2248,7 +2616,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" type="pres">
-      <dgm:prSet presAssocID="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="7" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="8" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2271,7 +2639,7 @@
       <dgm:spPr/>
     </dgm:pt>
     <dgm:pt modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}" type="pres">
-      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootText" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="8">
+      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootText" presStyleLbl="node3" presStyleIdx="8" presStyleCnt="10">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2286,7 +2654,7 @@
       </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8D67E224-0EDF-448A-9790-7C530F95D644}" type="pres">
-      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="7" presStyleCnt="8"/>
+      <dgm:prSet presAssocID="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="8" presStyleCnt="10"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2422,31 +2790,24 @@
       <dgm:prSet presAssocID="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" presName="hierChild5" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" type="pres">
-      <dgm:prSet presAssocID="{CEED879D-C918-490C-A079-5102097205A7}" presName="Name64" presStyleLbl="parChTrans1D2" presStyleIdx="6" presStyleCnt="7"/>
-      <dgm:spPr/>
-      <dgm:t>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
-        </a:p>
-      </dgm:t>
-    </dgm:pt>
-    <dgm:pt modelId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" type="pres">
-      <dgm:prSet presAssocID="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" presName="hierRoot2" presStyleCnt="0">
+    <dgm:pt modelId="{4ACAA18A-FBAA-4144-A54E-57F8DC1C473C}" type="pres">
+      <dgm:prSet presAssocID="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" presName="hierChild3" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E8A50146-44D3-4F0D-9944-35F07B49FA15}" type="pres">
+      <dgm:prSet presAssocID="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" presName="hierRoot1" presStyleCnt="0">
         <dgm:presLayoutVars>
           <dgm:hierBranch val="init"/>
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
     </dgm:pt>
-    <dgm:pt modelId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" type="pres">
-      <dgm:prSet presAssocID="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" presName="rootComposite" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}" type="pres">
-      <dgm:prSet presAssocID="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" presName="rootText" presStyleLbl="node2" presStyleIdx="6" presStyleCnt="7">
+    <dgm:pt modelId="{258AEF5F-94E7-49E5-B45D-86BBBF395A55}" type="pres">
+      <dgm:prSet presAssocID="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" presName="rootComposite1" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{29399504-D2C7-4F6F-AF1C-8ACC2C7B5F96}" type="pres">
+      <dgm:prSet presAssocID="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" presName="rootText1" presStyleLbl="node0" presStyleIdx="1" presStyleCnt="2">
         <dgm:presLayoutVars>
           <dgm:chPref val="3"/>
         </dgm:presLayoutVars>
@@ -2460,8 +2821,8 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" type="pres">
-      <dgm:prSet presAssocID="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="6" presStyleCnt="7"/>
+    <dgm:pt modelId="{050AEA4B-D93B-41FF-8434-E54219DBF300}" type="pres">
+      <dgm:prSet presAssocID="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" presName="rootConnector1" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="0"/>
       <dgm:spPr/>
       <dgm:t>
         <a:bodyPr/>
@@ -2471,84 +2832,299 @@
         </a:p>
       </dgm:t>
     </dgm:pt>
-    <dgm:pt modelId="{4AEBA50B-F3AB-455F-808A-6D8D6F6C8FC7}" type="pres">
-      <dgm:prSet presAssocID="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" presName="hierChild4" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{47D9F871-9894-4842-A60A-C9A1F58C3CB5}" type="pres">
-      <dgm:prSet presAssocID="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" presName="hierChild5" presStyleCnt="0"/>
-      <dgm:spPr/>
-    </dgm:pt>
-    <dgm:pt modelId="{4ACAA18A-FBAA-4144-A54E-57F8DC1C473C}" type="pres">
-      <dgm:prSet presAssocID="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" presName="hierChild3" presStyleCnt="0"/>
+    <dgm:pt modelId="{75E941CB-D0F4-47A9-81D0-6B014BDFEC85}" type="pres">
+      <dgm:prSet presAssocID="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" presName="hierChild2" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{525C1C18-1E95-47D9-936A-CDC62511FB07}" type="pres">
+      <dgm:prSet presAssocID="{C10D3E82-F9A1-462C-8FBA-5BD8E7806F8E}" presName="Name64" presStyleLbl="parChTrans1D2" presStyleIdx="6" presStyleCnt="7"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5A5AF78F-94BC-4F72-B04B-AA02D9CABE93}" type="pres">
+      <dgm:prSet presAssocID="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{41205725-97E6-4B5C-B2C5-942FAD02E850}" type="pres">
+      <dgm:prSet presAssocID="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8D36FDD9-C4A3-439F-8065-9CD5119A8A1D}" type="pres">
+      <dgm:prSet presAssocID="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" presName="rootText" presStyleLbl="node2" presStyleIdx="6" presStyleCnt="7">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{962BF409-2029-46E4-AD53-C9B88EA11444}" type="pres">
+      <dgm:prSet presAssocID="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" presName="rootConnector" presStyleLbl="node2" presStyleIdx="6" presStyleCnt="7"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A416A99A-2E86-4071-9BB0-C82F3662BB15}" type="pres">
+      <dgm:prSet presAssocID="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{7ABFFC0D-740C-4B29-AD4D-33E87F0E3ADD}" type="pres">
+      <dgm:prSet presAssocID="{D6DCACAB-7D92-46B6-A2ED-8043909D48F3}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="10"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{98628486-4CE5-4842-B931-3C49C481B35B}" type="pres">
+      <dgm:prSet presAssocID="{0FE1D759-A2B0-4446-9D87-B95385F80179}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{A2297BB1-00EB-482A-B3E0-1AFC8D029B59}" type="pres">
+      <dgm:prSet presAssocID="{0FE1D759-A2B0-4446-9D87-B95385F80179}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E167FCA0-7961-4302-99E1-B15A3C1C0377}" type="pres">
+      <dgm:prSet presAssocID="{0FE1D759-A2B0-4446-9D87-B95385F80179}" presName="rootText" presStyleLbl="node3" presStyleIdx="9" presStyleCnt="10">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{CF000C59-7C80-47D6-BB48-DE42227A607D}" type="pres">
+      <dgm:prSet presAssocID="{0FE1D759-A2B0-4446-9D87-B95385F80179}" presName="rootConnector" presStyleLbl="node3" presStyleIdx="9" presStyleCnt="10"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{E9298E38-E4FA-4009-8616-F7A604E18C7F}" type="pres">
+      <dgm:prSet presAssocID="{0FE1D759-A2B0-4446-9D87-B95385F80179}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5A3D3ADE-65DD-4A97-9D37-14548E59672B}" type="pres">
+      <dgm:prSet presAssocID="{DA47D477-365A-4A74-AA96-5E5FEB632109}" presName="Name64" presStyleLbl="parChTrans1D4" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B33B3A64-A2D1-4FDF-95D1-18EE677C1D5B}" type="pres">
+      <dgm:prSet presAssocID="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C298CB75-CF9F-4DBF-A558-B445BB6ACC0E}" type="pres">
+      <dgm:prSet presAssocID="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3AD42AA0-D75A-4389-96E7-C60023E6261B}" type="pres">
+      <dgm:prSet presAssocID="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" presName="rootText" presStyleLbl="node4" presStyleIdx="0" presStyleCnt="2">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3EFE6926-A7A5-4222-BA1F-A720C28229CD}" type="pres">
+      <dgm:prSet presAssocID="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" presName="rootConnector" presStyleLbl="node4" presStyleIdx="0" presStyleCnt="2"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A9A340B1-36CC-4F2C-B487-F55332995574}" type="pres">
+      <dgm:prSet presAssocID="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{378BE822-37E6-4E09-9C01-8504E675B5C7}" type="pres">
+      <dgm:prSet presAssocID="{B2F685BA-1AC9-4C10-A5F5-3E7531009405}" presName="Name64" presStyleLbl="parChTrans1D4" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5AF27C3A-2C7A-4CEF-8400-0C492FA94EDD}" type="pres">
+      <dgm:prSet presAssocID="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" presName="hierRoot2" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:hierBranch val="init"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C3B92546-78C1-40EF-9AF7-BDDEF279E2DB}" type="pres">
+      <dgm:prSet presAssocID="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{2D16E66E-9349-4E5D-B7C0-3011230746DB}" type="pres">
+      <dgm:prSet presAssocID="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" presName="rootText" presStyleLbl="node4" presStyleIdx="1" presStyleCnt="2">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="3"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C8F3EBB4-2268-4A43-A041-DF5281529549}" type="pres">
+      <dgm:prSet presAssocID="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" presName="rootConnector" presStyleLbl="node4" presStyleIdx="1" presStyleCnt="2"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B62C3081-E96A-4915-A25E-7DD752BEB701}" type="pres">
+      <dgm:prSet presAssocID="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" presName="hierChild4" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{BE0DE87F-21DC-4756-A621-A1DA61B5B87F}" type="pres">
+      <dgm:prSet presAssocID="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1EF885F5-99CB-48BD-A650-F968AABBD77D}" type="pres">
+      <dgm:prSet presAssocID="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D4374359-F403-45E7-A681-14ED46B48F1F}" type="pres">
+      <dgm:prSet presAssocID="{0FE1D759-A2B0-4446-9D87-B95385F80179}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{ADCCEFC3-34BD-4E7C-B04E-D61F5488475E}" type="pres">
+      <dgm:prSet presAssocID="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" presName="hierChild5" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{93E92B11-2646-4DEB-9FCB-34BE5730B31A}" type="pres">
+      <dgm:prSet presAssocID="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" presName="hierChild3" presStyleCnt="0"/>
       <dgm:spPr/>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
-    <dgm:cxn modelId="{7B55AD7D-CC95-45FE-BCFE-7B483051B4CB}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{559ADFF3-0478-496C-AFD5-D9545B790EC4}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FA5FD46B-9D83-45A4-9344-56D6066107F5}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{41CA1BF9-89DB-4278-B409-6043DE03BEF5}" type="presOf" srcId="{0FE1D759-A2B0-4446-9D87-B95385F80179}" destId="{E167FCA0-7961-4302-99E1-B15A3C1C0377}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1B7EE4ED-C343-4DBF-8592-DAF824F32B4F}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{5AD42C2B-3B72-4332-8CB0-CB02483CBB7A}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{39C1A42F-A2B3-466A-86DD-D4AFBF7A1403}" type="presOf" srcId="{A1986176-DBC3-405D-9BBF-0DA05F670219}" destId="{B364BDD2-2468-482C-B4F5-1A0AB60AF7B9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{0A3BCE5E-23D3-4914-A0DE-4D82B34706DE}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" srcOrd="0" destOrd="0" parTransId="{CCD73AB5-5FAC-49DE-B051-A16352DE18B0}" sibTransId="{90EBE641-EF69-4D14-98EF-9FFC06AA100B}"/>
+    <dgm:cxn modelId="{320201D6-8AE1-4176-9635-D81197B9E8AD}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1103E670-28FF-4AB2-9FAA-8999DB660777}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" srcOrd="1" destOrd="0" parTransId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" sibTransId="{0F39B1C9-85F1-4DD3-8B99-1EDD809C502C}"/>
+    <dgm:cxn modelId="{6DB29CA3-84E3-4AE3-B269-0E4E9A2370AB}" type="presOf" srcId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" destId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{41EA2324-B53B-4930-BACB-AFDEA8715A7A}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6EF22229-7E04-4838-8B5A-94EA53A1605C}" srcId="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" destId="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" srcOrd="0" destOrd="0" parTransId="{C10D3E82-F9A1-462C-8FBA-5BD8E7806F8E}" sibTransId="{332702D0-9CA2-4E0B-A3FB-CA3318461BBD}"/>
+    <dgm:cxn modelId="{215983E4-081D-4467-A756-55FEF443A562}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{C3C376ED-00F7-4F5C-BA18-766D538465C0}" type="presOf" srcId="{A1986176-DBC3-405D-9BBF-0DA05F670219}" destId="{C375CBC5-A09F-4275-BCD3-62BA4354A038}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{730324F8-2083-4C5C-9407-282C7ECD6870}" type="presOf" srcId="{C10D3E82-F9A1-462C-8FBA-5BD8E7806F8E}" destId="{525C1C18-1E95-47D9-936A-CDC62511FB07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{815260D8-FCB5-45E3-8AFB-F460679B2CDE}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{63A697A5-BE9C-4F91-A92C-3506C14F0A22}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2415E457-D5E9-475F-B3CE-4993C41B9B2A}" type="presOf" srcId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" destId="{9451D74F-6692-4FF1-A580-5574CD4401DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{32C55363-4473-460E-A765-20AB775E2E35}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{59FE6735-841D-4A73-8C46-6AEEC19B100C}" type="presOf" srcId="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" destId="{3EFE6926-A7A5-4222-BA1F-A720C28229CD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{EED1F78C-85BA-4908-9EDB-040048925EE2}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" srcOrd="0" destOrd="0" parTransId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" sibTransId="{D18382C1-3316-401F-B9F7-5740273EBE35}"/>
+    <dgm:cxn modelId="{752DC3CA-1459-43DF-8D17-59075C9B7B68}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B018499B-3C7A-4187-93DF-628C37B99276}" type="presOf" srcId="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" destId="{2D16E66E-9349-4E5D-B7C0-3011230746DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{5A36F1D5-ADA8-4676-90C2-A631BEDBF7F7}" type="presOf" srcId="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" destId="{8D36FDD9-C4A3-439F-8065-9CD5119A8A1D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{83B3D6F2-C63A-4120-828B-5A15440C2D24}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F5416D48-C226-4944-A1DE-B8EE2E87FE6D}" srcId="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" destId="{0FE1D759-A2B0-4446-9D87-B95385F80179}" srcOrd="0" destOrd="0" parTransId="{D6DCACAB-7D92-46B6-A2ED-8043909D48F3}" sibTransId="{2A7A3AB8-E3AE-4CC4-8537-EDB1BCE1615B}"/>
+    <dgm:cxn modelId="{D01C7126-32B6-4DB4-833B-0C12061AE485}" type="presOf" srcId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" destId="{224BDC60-7934-422F-B29C-84F028B56716}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FC7B3FFE-23C2-480C-9156-521BA5E4ED21}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{B7442801-F217-4912-AE49-8224D444B7AE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{47E9E0D7-561B-4062-99B9-8E5422CA1060}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{FE9E3000-93A4-4B79-A18F-D60B82D46552}" type="presOf" srcId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{BEE184DB-6F27-4D7A-9C18-98A0A01EDA70}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7BDC27E4-38E1-44C6-9275-7D0DAB391DBF}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D8ED3677-8BE0-47AD-826F-58E9D454D3D0}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" srcOrd="2" destOrd="0" parTransId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" sibTransId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}"/>
     <dgm:cxn modelId="{33CBFE4F-047C-4EDF-8FBC-62953BACFD7B}" type="presOf" srcId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" destId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{215983E4-081D-4467-A756-55FEF443A562}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6896BC00-BFB7-41F8-B6EF-61C2D24ED45E}" type="presOf" srcId="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" destId="{C8F3EBB4-2268-4A43-A041-DF5281529549}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7AC678BE-C1B9-4C2C-BBA5-63C6027EC514}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{C3D64037-6DDC-4D5F-B733-181307ADAF7C}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" srcOrd="1" destOrd="0" parTransId="{D95BA311-15D4-4B2B-A05D-399473AB7692}" sibTransId="{9915E53F-B0E6-44B6-B27E-B4A79CB3FBF7}"/>
+    <dgm:cxn modelId="{95DEC58E-CCCE-4EB2-8D93-F883B57FB55D}" type="presOf" srcId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" destId="{CDDBF60B-A81F-49D1-8951-61E79769BB23}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{35A1554D-6075-49F2-94F5-D41A56B41CB3}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" srcOrd="1" destOrd="0" parTransId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" sibTransId="{457716A4-F71B-4FD3-8107-7455FE567B34}"/>
+    <dgm:cxn modelId="{F81BCEF8-A95C-4677-921D-E34E2D2B1F37}" srcId="{0FE1D759-A2B0-4446-9D87-B95385F80179}" destId="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" srcOrd="0" destOrd="0" parTransId="{DA47D477-365A-4A74-AA96-5E5FEB632109}" sibTransId="{A56D162B-A8BF-4EE0-8EC5-7AA0A05D36B3}"/>
+    <dgm:cxn modelId="{DC212456-5040-4495-9F5E-3AA3C3560C20}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B9E26008-760E-4F53-A157-28E1F48ABE00}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" srcOrd="0" destOrd="0" parTransId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" sibTransId="{0F0D26FC-9E72-450A-A689-3301417EC882}"/>
+    <dgm:cxn modelId="{DE057FFD-529A-4E2E-B498-BC5F7742815B}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{078BFD8E-7E7A-44CB-8C2A-862AA6B7EF64}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{D823C5EF-1423-4863-AAC0-3CCB22E52AE5}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" srcOrd="0" destOrd="0" parTransId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" sibTransId="{EA4D083E-0312-47CC-8039-9496D55CDBDC}"/>
+    <dgm:cxn modelId="{97FB1D32-8AB3-45A8-8D63-292929166F76}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" srcOrd="1" destOrd="0" parTransId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" sibTransId="{2AD778EF-0F85-4883-B9FB-FEB9810673D5}"/>
+    <dgm:cxn modelId="{3F8AEC38-DCAC-422E-BBE1-60F8D32065DD}" type="presOf" srcId="{16684A72-88D1-4068-9742-A287A1AF7991}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E929C590-2797-4F5F-A36A-48FC41BCAC3F}" type="presOf" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{38BB76FF-0FA4-4F6D-A1F3-00F631A74DDB}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" srcOrd="3" destOrd="0" parTransId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" sibTransId="{DA3E9CE7-349A-4E9E-BD8A-D3E3EE2D990C}"/>
+    <dgm:cxn modelId="{C5ADD361-091A-4ECF-8689-E6A3B7125DA0}" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{A1986176-DBC3-405D-9BBF-0DA05F670219}" srcOrd="0" destOrd="0" parTransId="{5D3DE17C-EE5A-47BA-A905-F53770A94AE5}" sibTransId="{67DC55F0-7DFC-4F67-9A85-893F8218F853}"/>
+    <dgm:cxn modelId="{AD187AFA-F1B3-417B-A18B-1DA461641B00}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2135CB57-A821-4A45-B869-6D0CF021FCED}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" srcOrd="4" destOrd="0" parTransId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" sibTransId="{49B5EA05-D380-4B41-9D7A-E2087005D6BD}"/>
+    <dgm:cxn modelId="{BB4B00DC-A343-4429-9992-C97EBA76F0AA}" type="presOf" srcId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E1971364-B9C9-4F2D-8D2C-1C3FFC969523}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" srcOrd="2" destOrd="0" parTransId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" sibTransId="{12ED1614-9395-4694-B66E-BE7517C9B3C3}"/>
+    <dgm:cxn modelId="{6FF0C39F-4654-4B71-9CCA-06CDFB091AFF}" type="presOf" srcId="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" destId="{3AD42AA0-D75A-4389-96E7-C60023E6261B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="2" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
+    <dgm:cxn modelId="{F30AFEB2-A830-4035-BA71-EB491C42489C}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" srcOrd="0" destOrd="0" parTransId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" sibTransId="{E8DF5D1F-4EAF-4749-95FB-4BF5DDF36D94}"/>
     <dgm:cxn modelId="{0B25676A-30F3-4EC1-A0B7-586CBD08E376}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{28369DE3-437A-4135-B55E-48F1D6296DC6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{559ADFF3-0478-496C-AFD5-D9545B790EC4}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{B9E26008-760E-4F53-A157-28E1F48ABE00}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" srcOrd="0" destOrd="0" parTransId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" sibTransId="{0F0D26FC-9E72-450A-A689-3301417EC882}"/>
-    <dgm:cxn modelId="{EED1F78C-85BA-4908-9EDB-040048925EE2}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" srcOrd="0" destOrd="0" parTransId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" sibTransId="{D18382C1-3316-401F-B9F7-5740273EBE35}"/>
     <dgm:cxn modelId="{442C35E7-9219-42B1-8589-CA6B5AFD7FD1}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" srcOrd="5" destOrd="0" parTransId="{16684A72-88D1-4068-9742-A287A1AF7991}" sibTransId="{E1FF0606-7FA7-4C21-8E5B-4C259D042C61}"/>
+    <dgm:cxn modelId="{4B30A3EB-633B-43BD-9A9C-7AC22525B383}" type="presOf" srcId="{D6DCACAB-7D92-46B6-A2ED-8043909D48F3}" destId="{7ABFFC0D-740C-4B29-AD4D-33E87F0E3ADD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1C8DA176-6832-4A0E-81F3-4837C501AC26}" type="presOf" srcId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" destId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{DF818A78-A561-4994-847C-2D64179E539E}" type="presOf" srcId="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" destId="{962BF409-2029-46E4-AD53-C9B88EA11444}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{3E8883EC-AF64-4F90-8EBF-B7F2F7D2637C}" type="presOf" srcId="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" destId="{050AEA4B-D93B-41FF-8434-E54219DBF300}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{71DBFE96-B81B-465F-9F92-6E34F83D6304}" type="presOf" srcId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{38DBDA98-E1B6-4DF0-B945-0EC585B5EFB9}" type="presOf" srcId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" destId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{4B5EE178-606B-42A4-B57D-4F101E6DD6DB}" type="presOf" srcId="{5D3DE17C-EE5A-47BA-A905-F53770A94AE5}" destId="{1A2B8F52-9746-463C-BC4A-04A1B691DD53}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{64C51D7A-7313-43E7-BF9D-F942E1C38539}" type="presOf" srcId="{DA47D477-365A-4A74-AA96-5E5FEB632109}" destId="{5A3D3ADE-65DD-4A97-9D37-14548E59672B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{4DC23858-37C8-4751-B013-C8B89E1C790A}" type="presOf" srcId="{B2F685BA-1AC9-4C10-A5F5-3E7531009405}" destId="{378BE822-37E6-4E09-9C01-8504E675B5C7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E77DC00F-1DBC-4305-A75A-CA0AF88B6519}" type="presOf" srcId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" destId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9F01A4C8-FCDC-41BC-898B-747FEC5B6389}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B0C83AA9-272C-4A44-AC90-24DE78B5CC49}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{8AC7FAB9-3355-47AA-A457-7136F862B206}" srcId="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" destId="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" srcOrd="0" destOrd="0" parTransId="{B2F685BA-1AC9-4C10-A5F5-3E7531009405}" sibTransId="{AFFCDD44-5217-4C68-A5FA-27C9C7E1E33C}"/>
+    <dgm:cxn modelId="{1117B828-D277-43FA-B244-6FF95B68193E}" type="presOf" srcId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F5EBD142-F152-4BD8-AE52-4066178EEE6D}" type="presOf" srcId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{56247623-20AE-45E9-A8C5-000B0DE85F7F}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{82F277AB-87C7-433B-862F-87C13847027E}" srcOrd="1" destOrd="0" parTransId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" sibTransId="{8C3C1181-DF4B-4EE3-9ED3-562C8BC3A0A0}"/>
+    <dgm:cxn modelId="{6BFC3B2E-0155-4C03-A497-DE8D2EEF6C33}" type="presOf" srcId="{0FE1D759-A2B0-4446-9D87-B95385F80179}" destId="{CF000C59-7C80-47D6-BB48-DE42227A607D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{814C55A4-746A-46AC-B71C-48916393BAC3}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{F5B18884-E498-499B-92AD-14DA40157B0A}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E77DC00F-1DBC-4305-A75A-CA0AF88B6519}" type="presOf" srcId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" destId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{7AC678BE-C1B9-4C2C-BBA5-63C6027EC514}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{3188130F-D86D-4C20-8DED-588A1E2059A5}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{2415E457-D5E9-475F-B3CE-4993C41B9B2A}" type="presOf" srcId="{86B5CE75-F3EF-4F68-89EE-8C209B2194B9}" destId="{9451D74F-6692-4FF1-A580-5574CD4401DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F5EBD142-F152-4BD8-AE52-4066178EEE6D}" type="presOf" srcId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" destId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{1C8DA176-6832-4A0E-81F3-4837C501AC26}" type="presOf" srcId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" destId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{DE057FFD-529A-4E2E-B498-BC5F7742815B}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{078BFD8E-7E7A-44CB-8C2A-862AA6B7EF64}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{42202B6F-09AF-469F-BAF4-B48BCDFB8F97}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" srcOrd="1" destOrd="0" parTransId="{0F80066D-D524-4CD9-99A1-9E2B131A7B29}" sibTransId="{457716A4-F71B-4FD3-8107-7455FE567B34}"/>
-    <dgm:cxn modelId="{1B7EE4ED-C343-4DBF-8592-DAF824F32B4F}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{35A1554D-6075-49F2-94F5-D41A56B41CB3}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{BEE184DB-6F27-4D7A-9C18-98A0A01EDA70}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{F30AFEB2-A830-4035-BA71-EB491C42489C}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" srcOrd="0" destOrd="0" parTransId="{B17096AB-13EE-436C-8A2F-D002B1DA64DD}" sibTransId="{E8DF5D1F-4EAF-4749-95FB-4BF5DDF36D94}"/>
-    <dgm:cxn modelId="{97FB1D32-8AB3-45A8-8D63-292929166F76}" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" srcOrd="1" destOrd="0" parTransId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" sibTransId="{2AD778EF-0F85-4883-B9FB-FEB9810673D5}"/>
-    <dgm:cxn modelId="{2135CB57-A821-4A45-B869-6D0CF021FCED}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" srcOrd="4" destOrd="0" parTransId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" sibTransId="{49B5EA05-D380-4B41-9D7A-E2087005D6BD}"/>
-    <dgm:cxn modelId="{815260D8-FCB5-45E3-8AFB-F460679B2CDE}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D0A170FC-0AB5-4AEF-91B1-1D414CCEFE41}" type="presOf" srcId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{92107E38-7630-470C-9791-C19A37DEC9FA}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{B2A681BD-5EE0-45B6-B4F9-016D77485296}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{9F01A4C8-FCDC-41BC-898B-747FEC5B6389}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{1117B828-D277-43FA-B244-6FF95B68193E}" type="presOf" srcId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{38BB76FF-0FA4-4F6D-A1F3-00F631A74DDB}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" srcOrd="3" destOrd="0" parTransId="{18C42E23-C3B3-4C8F-AF05-44033742F50B}" sibTransId="{DA3E9CE7-349A-4E9E-BD8A-D3E3EE2D990C}"/>
-    <dgm:cxn modelId="{D01C7126-32B6-4DB4-833B-0C12061AE485}" type="presOf" srcId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" destId="{224BDC60-7934-422F-B29C-84F028B56716}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{752DC3CA-1459-43DF-8D17-59075C9B7B68}" type="presOf" srcId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" destId="{F5DF627C-D57A-429A-ACDC-8DBDE2024C3D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AB607608-F446-4589-976E-8D4BC4235A8D}" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{53B6DBC8-7410-4D20-AB8F-1DDC8B938080}" srcOrd="2" destOrd="0" parTransId="{E3CC51D3-BA61-42DC-BE60-BC36B01B7288}" sibTransId="{2C9CDD52-F136-461F-866B-9F21BD094A9F}"/>
-    <dgm:cxn modelId="{32C55363-4473-460E-A765-20AB775E2E35}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{DC212456-5040-4495-9F5E-3AA3C3560C20}" type="presOf" srcId="{629E773C-EE7D-482A-94D1-6BB3211F734D}" destId="{86208CCA-CF72-4B42-BD30-1CF44C6EDEAD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{FE9E3000-93A4-4B79-A18F-D60B82D46552}" type="presOf" srcId="{C11E542B-9992-4C4A-BE7E-55D246AAC2D9}" destId="{94834600-2A81-4D2E-BA8C-D171F42E9531}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{6B143136-E6DE-46E8-9AD5-1977D53BF989}" type="presOf" srcId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" destId="{0FAB1775-08F8-482E-A204-647B49CA8593}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{320201D6-8AE1-4176-9635-D81197B9E8AD}" type="presOf" srcId="{D683009A-7397-46BB-ACEC-EF0F80D516C9}" destId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{56247623-20AE-45E9-A8C5-000B0DE85F7F}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{82F277AB-87C7-433B-862F-87C13847027E}" srcOrd="1" destOrd="0" parTransId="{BBD94F22-B40F-4F52-86AD-C131913DD102}" sibTransId="{8C3C1181-DF4B-4EE3-9ED3-562C8BC3A0A0}"/>
-    <dgm:cxn modelId="{E929C590-2797-4F5F-A36A-48FC41BCAC3F}" type="presOf" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{FC7B3FFE-23C2-480C-9156-521BA5E4ED21}" type="presOf" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{B7442801-F217-4912-AE49-8224D444B7AE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{0A3BCE5E-23D3-4914-A0DE-4D82B34706DE}" srcId="{0AACF41D-7981-4393-B317-C2E0308F1883}" destId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" srcOrd="0" destOrd="0" parTransId="{CCD73AB5-5FAC-49DE-B051-A16352DE18B0}" sibTransId="{90EBE641-EF69-4D14-98EF-9FFC06AA100B}"/>
-    <dgm:cxn modelId="{95DEC58E-CCCE-4EB2-8D93-F883B57FB55D}" type="presOf" srcId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" destId="{CDDBF60B-A81F-49D1-8951-61E79769BB23}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D0A170FC-0AB5-4AEF-91B1-1D414CCEFE41}" type="presOf" srcId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" destId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{6DB29CA3-84E3-4AE3-B269-0E4E9A2370AB}" type="presOf" srcId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" destId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{3F8AEC38-DCAC-422E-BBE1-60F8D32065DD}" type="presOf" srcId="{16684A72-88D1-4068-9742-A287A1AF7991}" destId="{400A970B-01E2-495E-9ECB-7EADDBB33666}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{5AD42C2B-3B72-4332-8CB0-CB02483CBB7A}" type="presOf" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AD187AFA-F1B3-417B-A18B-1DA461641B00}" type="presOf" srcId="{7C91B66F-713C-4590-8ADA-F8886C035DD3}" destId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{BB4B00DC-A343-4429-9992-C97EBA76F0AA}" type="presOf" srcId="{CC820015-08D8-4836-A31C-2D63FBA54C31}" destId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{47E9E0D7-561B-4062-99B9-8E5422CA1060}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{1103E670-28FF-4AB2-9FAA-8999DB660777}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" srcOrd="1" destOrd="0" parTransId="{309C8B67-9DEE-48CF-AD25-08567C3E78A9}" sibTransId="{0F39B1C9-85F1-4DD3-8B99-1EDD809C502C}"/>
-    <dgm:cxn modelId="{63A697A5-BE9C-4F91-A92C-3506C14F0A22}" type="presOf" srcId="{29C292E2-1E5B-4094-B0FF-39F7CCD79699}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{D8ED3677-8BE0-47AD-826F-58E9D454D3D0}" type="presOf" srcId="{315A1BF6-352E-41EB-A8FF-22EFE8BC0429}" destId="{0AEF7E3D-FD04-4C6B-A013-9C9ACD8AB4FA}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{8E74C319-B9D0-46CC-A8A4-BF750DD4159D}" type="presOf" srcId="{C717E33D-3BF3-4CA1-8059-DAE33C38EA14}" destId="{29399504-D2C7-4F6F-AF1C-8ACC2C7B5F96}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{C1D1B42F-A616-40D8-84DC-A1AD40C3E0D0}" type="presOf" srcId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" destId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{1C6CD132-06CD-4B2C-8DDD-553AE71D597C}" type="presOf" srcId="{BA8AC38B-EF15-4E8A-9C84-A3689DC24C69}" destId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{B0C83AA9-272C-4A44-AC90-24DE78B5CC49}" type="presOf" srcId="{38BE8CCA-B84F-4FB7-B448-A5C162873B23}" destId="{8D67E224-0EDF-448A-9790-7C530F95D644}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{83B3D6F2-C63A-4120-828B-5A15440C2D24}" type="presOf" srcId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{404FFDC8-1807-40B1-88B3-D52B6630D710}" type="presOf" srcId="{CEED879D-C918-490C-A079-5102097205A7}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{85ED09CB-BBA9-44F9-A7D1-0AA0918F400D}" srcId="{82F277AB-87C7-433B-862F-87C13847027E}" destId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" srcOrd="2" destOrd="0" parTransId="{C72AEC07-F53B-4926-9FF1-882AD3C02EC1}" sibTransId="{C45B34A5-4124-453B-80CE-B08FF7C0D403}"/>
-    <dgm:cxn modelId="{FA5FD46B-9D83-45A4-9344-56D6066107F5}" type="presOf" srcId="{01E7DD4F-A7E0-4388-B91D-5E6C63A54884}" destId="{0728688F-C177-4E5E-A4EB-C5D5E7BE790E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{7BDC27E4-38E1-44C6-9275-7D0DAB391DBF}" type="presOf" srcId="{CD110BC5-A6EE-425E-A4FC-47E303EA6724}" destId="{9AF49657-AA78-4094-A9BE-88522ADD0F43}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{C1D1B42F-A616-40D8-84DC-A1AD40C3E0D0}" type="presOf" srcId="{97A37FF1-B7D0-4136-AD7A-708319E220BF}" destId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AA066BC1-D6A6-463C-AFF2-1173ECB16332}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{D0334CD6-80CA-401B-8CA3-883E08A430DA}" srcOrd="6" destOrd="0" parTransId="{CEED879D-C918-490C-A079-5102097205A7}" sibTransId="{96D318EA-92A6-4D06-8BD0-F3437FB33BA9}"/>
-    <dgm:cxn modelId="{38DBDA98-E1B6-4DF0-B945-0EC585B5EFB9}" type="presOf" srcId="{4C9914D3-4F08-444F-865A-47F48A3FFB6B}" destId="{6390FF4A-F0A9-4F65-975E-14F195A61516}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{71DBFE96-B81B-465F-9F92-6E34F83D6304}" type="presOf" srcId="{B981D15F-796C-4F03-AEDF-FD448CA5C85B}" destId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E1971364-B9C9-4F2D-8D2C-1C3FFC969523}" srcId="{78CEA145-955C-4876-97BE-5F6C3FB3B1D4}" destId="{CCB51DA8-C62A-439F-B252-D6569840A52F}" srcOrd="2" destOrd="0" parTransId="{612E6167-3C1F-4A58-B33B-0E0EE02F8CF5}" sibTransId="{12ED1614-9395-4694-B66E-BE7517C9B3C3}"/>
-    <dgm:cxn modelId="{41EA2324-B53B-4930-BACB-AFDEA8715A7A}" type="presOf" srcId="{9019F039-A6BB-4811-9BF3-881F48EB4453}" destId="{4A648E3C-C261-416B-9C1F-302690AD5D33}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{2D7F7C22-ADD5-4E45-A535-C589EB253F20}" type="presParOf" srcId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" destId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{C9F10509-5022-4B9B-A341-CC3365CCCF88}" type="presParOf" srcId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" destId="{87B98112-BB49-47E9-92F1-82F9448578BD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{CDA112DB-C227-483A-BA50-1640272F1F9E}" type="presParOf" srcId="{87B98112-BB49-47E9-92F1-82F9448578BD}" destId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2616,6 +3192,13 @@
     <dgm:cxn modelId="{E977C6FF-7906-45F1-903A-F572CE9B3D3B}" type="presParOf" srcId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" destId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{234AC40D-7A12-4A42-8747-1718EA8724EF}" type="presParOf" srcId="{DB7A36C6-32EA-44C1-980F-D3E4B66E6060}" destId="{2C590C59-0A51-4B0A-9E3F-B81519A71165}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{82A5785E-3DD7-4D75-84AE-00C846E6CA34}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{CF2FCF6C-326F-4DC9-B8A1-0BF6C9D81E44}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6DF45745-C26F-4E4B-B197-55E58E9AF2CF}" type="presParOf" srcId="{CF2FCF6C-326F-4DC9-B8A1-0BF6C9D81E44}" destId="{1A2B8F52-9746-463C-BC4A-04A1B691DD53}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2B609804-B347-4555-A322-D880766377F2}" type="presParOf" srcId="{CF2FCF6C-326F-4DC9-B8A1-0BF6C9D81E44}" destId="{9F313496-2623-4AFE-A6FB-DA38AFC23721}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{042742B5-003E-4E5F-8CE2-3637BBCA06B7}" type="presParOf" srcId="{9F313496-2623-4AFE-A6FB-DA38AFC23721}" destId="{5D39ABD7-8940-4EB0-BD28-24328861EAC2}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{5BC7A111-A60A-428B-AA56-FAC9E429EE58}" type="presParOf" srcId="{5D39ABD7-8940-4EB0-BD28-24328861EAC2}" destId="{B364BDD2-2468-482C-B4F5-1A0AB60AF7B9}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9ADA812B-7905-4CFA-9714-5DA886CB017A}" type="presParOf" srcId="{5D39ABD7-8940-4EB0-BD28-24328861EAC2}" destId="{C375CBC5-A09F-4275-BCD3-62BA4354A038}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{4366E6EB-8011-4D2D-9329-9AC956D59826}" type="presParOf" srcId="{9F313496-2623-4AFE-A6FB-DA38AFC23721}" destId="{EFA21C3A-FA62-4E09-874C-52C385FC8442}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{904A3AA8-F147-4FBA-A195-98E40742087D}" type="presParOf" srcId="{9F313496-2623-4AFE-A6FB-DA38AFC23721}" destId="{4966423A-AE1F-4EA5-97F1-80EF66672A6D}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{49DD7261-B542-4333-BBCD-7F647314647E}" type="presParOf" srcId="{E9CAD542-1CE1-4830-B7FC-D32E8C576386}" destId="{0179D0B3-6350-4D61-9B67-663CD880CA02}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{7DBE53AB-4C21-483C-A0DF-B2FDF0DDEA0C}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{E0568980-BD26-44B0-99C5-2B5582E6C423}" srcOrd="6" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{0D9B4DB5-A00D-4982-89A0-AD4E75620233}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{B01B4204-89ED-4030-B5B5-CA72D3696CAD}" srcOrd="7" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
@@ -2652,14 +3235,41 @@
     <dgm:cxn modelId="{F4F38111-0959-4E30-8E76-B27D793DFD08}" type="presParOf" srcId="{951A5EBE-973F-49D2-AEE8-E9C1FD21E621}" destId="{577389ED-C7E0-4902-B013-725B00096C99}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{A662CC20-B897-4C23-BE86-052F51FE0961}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{5154CB22-61FB-414C-948D-B5CAB376CD6A}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{9938CBB7-1955-4A14-9738-70EC3065762F}" type="presParOf" srcId="{14920BCF-0F77-45F3-AF09-5773FB403370}" destId="{E0CF165D-444F-4D0C-9894-0CEE601662E0}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AF9273E8-AF53-4499-B8EE-B157657049B7}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{FE068172-564A-4253-AF89-D2BDB64E74DA}" srcOrd="12" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{AEA0668E-5882-411E-A90E-9A18917A58B1}" type="presParOf" srcId="{2734E417-4FC0-4A6B-B0CC-CFAA9B95649C}" destId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" srcOrd="13" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{E22B93FF-C5B5-40D0-9D8C-30BF0BBC24DC}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{65890E10-58E8-4BB6-AC06-53B5F5902D6D}" type="presParOf" srcId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" destId="{0FAB1775-08F8-482E-A204-647B49CA8593}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{21E81E96-CA96-4354-BA05-52A08BD70467}" type="presParOf" srcId="{51FAB9D8-D314-4EF7-8106-90E0460FBCFB}" destId="{3FD4089E-682F-44D3-B177-E2503B9A71BD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{A1551817-5CA6-4336-800C-150B1652172E}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{4AEBA50B-F3AB-455F-808A-6D8D6F6C8FC7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
-    <dgm:cxn modelId="{DA3B8371-91A3-4863-94CB-876FC2B8007A}" type="presParOf" srcId="{35728C78-1066-402E-8B6C-A5E6D307DFC3}" destId="{47D9F871-9894-4842-A60A-C9A1F58C3CB5}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
     <dgm:cxn modelId="{403888BF-165D-4DF9-99BD-77EA280BF47C}" type="presParOf" srcId="{CD26FC17-709C-440D-945B-F2D12EF53DF2}" destId="{4ACAA18A-FBAA-4144-A54E-57F8DC1C473C}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{284B478C-5FF0-4B75-802C-0CF11A238619}" type="presParOf" srcId="{D7BF436B-0567-4F7D-9784-9BCB87E624EF}" destId="{E8A50146-44D3-4F0D-9944-35F07B49FA15}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{D0399142-9606-431C-91D5-18495BFC6552}" type="presParOf" srcId="{E8A50146-44D3-4F0D-9944-35F07B49FA15}" destId="{258AEF5F-94E7-49E5-B45D-86BBBF395A55}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{376264E6-6BB0-4C31-ABD3-C15D524B1596}" type="presParOf" srcId="{258AEF5F-94E7-49E5-B45D-86BBBF395A55}" destId="{29399504-D2C7-4F6F-AF1C-8ACC2C7B5F96}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{9EE94668-0AFD-4113-B06B-2A64A3860B6D}" type="presParOf" srcId="{258AEF5F-94E7-49E5-B45D-86BBBF395A55}" destId="{050AEA4B-D93B-41FF-8434-E54219DBF300}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{010EE6CC-5019-42EA-8713-7D4895ED27FE}" type="presParOf" srcId="{E8A50146-44D3-4F0D-9944-35F07B49FA15}" destId="{75E941CB-D0F4-47A9-81D0-6B014BDFEC85}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{14F2689A-D7D9-4572-9700-3F3098BC9419}" type="presParOf" srcId="{75E941CB-D0F4-47A9-81D0-6B014BDFEC85}" destId="{525C1C18-1E95-47D9-936A-CDC62511FB07}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{071EF61B-81CB-4055-8290-BBDE33D62C0F}" type="presParOf" srcId="{75E941CB-D0F4-47A9-81D0-6B014BDFEC85}" destId="{5A5AF78F-94BC-4F72-B04B-AA02D9CABE93}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{565FD345-8DE2-4150-8D11-17EC64BA9946}" type="presParOf" srcId="{5A5AF78F-94BC-4F72-B04B-AA02D9CABE93}" destId="{41205725-97E6-4B5C-B2C5-942FAD02E850}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{5FE5D3D1-71AD-45DE-A6AD-060E2808ADBF}" type="presParOf" srcId="{41205725-97E6-4B5C-B2C5-942FAD02E850}" destId="{8D36FDD9-C4A3-439F-8065-9CD5119A8A1D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{B113FB4A-EAB5-42AC-BCD2-4A19E92897DF}" type="presParOf" srcId="{41205725-97E6-4B5C-B2C5-942FAD02E850}" destId="{962BF409-2029-46E4-AD53-C9B88EA11444}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{08FDC6BB-0B43-46AB-82F1-2A54E4E7DBC4}" type="presParOf" srcId="{5A5AF78F-94BC-4F72-B04B-AA02D9CABE93}" destId="{A416A99A-2E86-4071-9BB0-C82F3662BB15}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2B776399-128D-4D87-8870-D8F2E83C04BD}" type="presParOf" srcId="{A416A99A-2E86-4071-9BB0-C82F3662BB15}" destId="{7ABFFC0D-740C-4B29-AD4D-33E87F0E3ADD}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1BB6CFBB-0632-4D9D-BE08-F2400FC30DC1}" type="presParOf" srcId="{A416A99A-2E86-4071-9BB0-C82F3662BB15}" destId="{98628486-4CE5-4842-B931-3C49C481B35B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{6A001030-DC54-4085-BA8A-B5EB1CDFE796}" type="presParOf" srcId="{98628486-4CE5-4842-B931-3C49C481B35B}" destId="{A2297BB1-00EB-482A-B3E0-1AFC8D029B59}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{82492E40-86FB-4126-AC89-33955EB79874}" type="presParOf" srcId="{A2297BB1-00EB-482A-B3E0-1AFC8D029B59}" destId="{E167FCA0-7961-4302-99E1-B15A3C1C0377}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{495A62FA-85CA-413F-AF3F-D9D20AE76FB5}" type="presParOf" srcId="{A2297BB1-00EB-482A-B3E0-1AFC8D029B59}" destId="{CF000C59-7C80-47D6-BB48-DE42227A607D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F101D7E5-DF1D-49DC-9C7D-50A6424F5C91}" type="presParOf" srcId="{98628486-4CE5-4842-B931-3C49C481B35B}" destId="{E9298E38-E4FA-4009-8616-F7A604E18C7F}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{E2C77F38-A94B-4362-8322-78B613D70D42}" type="presParOf" srcId="{E9298E38-E4FA-4009-8616-F7A604E18C7F}" destId="{5A3D3ADE-65DD-4A97-9D37-14548E59672B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2B39A74F-5ABB-467D-90D6-CB90F374E361}" type="presParOf" srcId="{E9298E38-E4FA-4009-8616-F7A604E18C7F}" destId="{B33B3A64-A2D1-4FDF-95D1-18EE677C1D5B}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{316D2683-7373-46A4-86DD-BB80787485E4}" type="presParOf" srcId="{B33B3A64-A2D1-4FDF-95D1-18EE677C1D5B}" destId="{C298CB75-CF9F-4DBF-A558-B445BB6ACC0E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{11FEFE54-E6F9-4199-BBBB-7439E6BF2CF0}" type="presParOf" srcId="{C298CB75-CF9F-4DBF-A558-B445BB6ACC0E}" destId="{3AD42AA0-D75A-4389-96E7-C60023E6261B}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{0E5152CD-96CC-4C6C-AEEB-1BAF8312857F}" type="presParOf" srcId="{C298CB75-CF9F-4DBF-A558-B445BB6ACC0E}" destId="{3EFE6926-A7A5-4222-BA1F-A720C28229CD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{90A014B5-C0EC-4283-93C4-8AA79F9A69AF}" type="presParOf" srcId="{B33B3A64-A2D1-4FDF-95D1-18EE677C1D5B}" destId="{A9A340B1-36CC-4F2C-B487-F55332995574}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{06EAAE10-E121-4BC2-B687-0ECB8A3D6596}" type="presParOf" srcId="{A9A340B1-36CC-4F2C-B487-F55332995574}" destId="{378BE822-37E6-4E09-9C01-8504E675B5C7}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{56019D86-6F6E-4848-BEC5-2C931170B1CA}" type="presParOf" srcId="{A9A340B1-36CC-4F2C-B487-F55332995574}" destId="{5AF27C3A-2C7A-4CEF-8400-0C492FA94EDD}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F24C5B83-6BBE-4102-A046-EF3DD3BAC8A1}" type="presParOf" srcId="{5AF27C3A-2C7A-4CEF-8400-0C492FA94EDD}" destId="{C3B92546-78C1-40EF-9AF7-BDDEF279E2DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{321AB5DC-A72A-464B-901C-9AFA70BEB7C6}" type="presParOf" srcId="{C3B92546-78C1-40EF-9AF7-BDDEF279E2DB}" destId="{2D16E66E-9349-4E5D-B7C0-3011230746DB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{7ADBB098-1597-4CD6-8FB8-17EEFB68A274}" type="presParOf" srcId="{C3B92546-78C1-40EF-9AF7-BDDEF279E2DB}" destId="{C8F3EBB4-2268-4A43-A041-DF5281529549}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{2A0D9A3B-EDA5-4F9B-A394-8D1DD446A9D3}" type="presParOf" srcId="{5AF27C3A-2C7A-4CEF-8400-0C492FA94EDD}" destId="{B62C3081-E96A-4915-A25E-7DD752BEB701}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{1F121C1D-A5DD-4720-9011-79A33D413CEF}" type="presParOf" srcId="{5AF27C3A-2C7A-4CEF-8400-0C492FA94EDD}" destId="{BE0DE87F-21DC-4756-A621-A1DA61B5B87F}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{86BDE1C2-0EBD-4288-96C8-C17F3FDBD452}" type="presParOf" srcId="{B33B3A64-A2D1-4FDF-95D1-18EE677C1D5B}" destId="{1EF885F5-99CB-48BD-A650-F968AABBD77D}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{CB5CB334-66FF-4FAF-B6E8-CA75193D113C}" type="presParOf" srcId="{98628486-4CE5-4842-B931-3C49C481B35B}" destId="{D4374359-F403-45E7-A681-14ED46B48F1F}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{EDEF1713-4FB9-49FD-A7A9-EE2C42966618}" type="presParOf" srcId="{5A5AF78F-94BC-4F72-B04B-AA02D9CABE93}" destId="{ADCCEFC3-34BD-4E7C-B04E-D61F5488475E}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
+    <dgm:cxn modelId="{F087E2A5-78B1-44C2-A6C4-2309CE765EC2}" type="presParOf" srcId="{E8A50146-44D3-4F0D-9944-35F07B49FA15}" destId="{93E92B11-2646-4DEB-9FCB-34BE5730B31A}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2009/3/layout/HorizontalOrganizationChart"/>
   </dgm:cxnLst>
   <dgm:bg/>
   <dgm:whole/>
@@ -2679,15 +3289,15 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
-    <dsp:sp modelId="{FE068172-564A-4253-AF89-D2BDB64E74DA}">
+    <dsp:sp modelId="{378BE822-37E6-4E09-9C01-8504E675B5C7}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3645556" y="2109676"/>
-          <a:ext cx="174891" cy="1598067"/>
+          <a:off x="5611716" y="3674036"/>
+          <a:ext cx="159298" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2698,16 +3308,175 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="0"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="159298" y="45720"/>
               </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{5A3D3ADE-65DD-4A97-9D37-14548E59672B}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4655922" y="3674036"/>
+          <a:ext cx="159298" cy="91440"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="45720"/>
+              </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="1598067"/>
+                <a:pt x="159298" y="45720"/>
               </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{7ABFFC0D-740C-4B29-AD4D-33E87F0E3ADD}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3700128" y="3674036"/>
+          <a:ext cx="159298" cy="91440"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="45720"/>
+              </a:moveTo>
               <a:lnTo>
-                <a:pt x="174891" y="1598067"/>
+                <a:pt x="159298" y="45720"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{525C1C18-1E95-47D9-936A-CDC62511FB07}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2744334" y="3674036"/>
+          <a:ext cx="159298" cy="91440"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="45720"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="159298" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2747,8 +3516,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3645556" y="2109676"/>
-          <a:ext cx="174891" cy="1222051"/>
+          <a:off x="2744334" y="1921669"/>
+          <a:ext cx="159298" cy="1455594"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2762,13 +3531,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="1222051"/>
+                <a:pt x="79649" y="1455594"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="1222051"/>
+                <a:pt x="159298" y="1455594"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2808,8 +3577,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3645556" y="2109676"/>
-          <a:ext cx="174891" cy="846035"/>
+          <a:off x="2744334" y="1921669"/>
+          <a:ext cx="159298" cy="1113101"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2823,13 +3592,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="846035"/>
+                <a:pt x="79649" y="1113101"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="846035"/>
+                <a:pt x="159298" y="1113101"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2869,8 +3638,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="2579696"/>
-          <a:ext cx="174891" cy="188007"/>
+          <a:off x="3700128" y="2692277"/>
+          <a:ext cx="159298" cy="171246"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2884,13 +3653,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="188007"/>
+                <a:pt x="79649" y="171246"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="188007"/>
+                <a:pt x="159298" y="171246"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2930,8 +3699,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="2391688"/>
-          <a:ext cx="174891" cy="188007"/>
+          <a:off x="3700128" y="2521031"/>
+          <a:ext cx="159298" cy="171246"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -2942,16 +3711,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="188007"/>
+                <a:pt x="0" y="171246"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="188007"/>
+                <a:pt x="79649" y="171246"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="0"/>
+                <a:pt x="159298" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -2991,8 +3760,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3645556" y="2109676"/>
-          <a:ext cx="174891" cy="470019"/>
+          <a:off x="2744334" y="1921669"/>
+          <a:ext cx="159298" cy="770608"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3006,13 +3775,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="470019"/>
+                <a:pt x="79649" y="770608"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="470019"/>
+                <a:pt x="159298" y="770608"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3045,15 +3814,15 @@
         <a:fontRef idx="minor"/>
       </dsp:style>
     </dsp:sp>
-    <dsp:sp modelId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}">
+    <dsp:sp modelId="{1A2B8F52-9746-463C-BC4A-04A1B691DD53}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3645556" y="2015672"/>
-          <a:ext cx="174891" cy="94003"/>
+          <a:off x="3700128" y="2132818"/>
+          <a:ext cx="159298" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3064,16 +3833,71 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="94003"/>
+                <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="94003"/>
+                <a:pt x="159298" y="45720"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="80000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2744334" y="1921669"/>
+          <a:ext cx="159298" cy="256869"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="256869"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="0"/>
+                <a:pt x="159298" y="256869"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3113,8 +3937,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="1639657"/>
-          <a:ext cx="174891" cy="376015"/>
+          <a:off x="3700128" y="1493552"/>
+          <a:ext cx="159298" cy="342492"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3128,13 +3952,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="376015"/>
+                <a:pt x="79649" y="342492"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="376015"/>
+                <a:pt x="159298" y="342492"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3174,8 +3998,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="1593937"/>
-          <a:ext cx="174891" cy="91440"/>
+          <a:off x="3700128" y="1447832"/>
+          <a:ext cx="159298" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3189,7 +4013,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="174891" y="45720"/>
+                <a:pt x="159298" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3229,8 +4053,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="1263641"/>
-          <a:ext cx="174891" cy="376015"/>
+          <a:off x="3700128" y="1151060"/>
+          <a:ext cx="159298" cy="342492"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3241,16 +4065,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="376015"/>
+                <a:pt x="0" y="342492"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="376015"/>
+                <a:pt x="79649" y="342492"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="0"/>
+                <a:pt x="159298" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3290,8 +4114,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3645556" y="1639657"/>
-          <a:ext cx="174891" cy="470019"/>
+          <a:off x="2744334" y="1493552"/>
+          <a:ext cx="159298" cy="428116"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3302,16 +4126,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="470019"/>
+                <a:pt x="0" y="428116"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="470019"/>
+                <a:pt x="79649" y="428116"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="0"/>
+                <a:pt x="159298" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3351,8 +4175,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="511609"/>
-          <a:ext cx="174891" cy="376015"/>
+          <a:off x="3700128" y="466074"/>
+          <a:ext cx="159298" cy="342492"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3366,13 +4190,13 @@
                 <a:pt x="0" y="0"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="376015"/>
+                <a:pt x="79649" y="342492"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="376015"/>
+                <a:pt x="159298" y="342492"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3412,8 +4236,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="465889"/>
-          <a:ext cx="174891" cy="91440"/>
+          <a:off x="3700128" y="420354"/>
+          <a:ext cx="159298" cy="91440"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3427,7 +4251,7 @@
                 <a:pt x="0" y="45720"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="174891" y="45720"/>
+                <a:pt x="159298" y="45720"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3467,8 +4291,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4694902" y="135593"/>
-          <a:ext cx="174891" cy="376015"/>
+          <a:off x="3700128" y="123581"/>
+          <a:ext cx="159298" cy="342492"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3479,16 +4303,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="376015"/>
+                <a:pt x="0" y="342492"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="376015"/>
+                <a:pt x="79649" y="342492"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="0"/>
+                <a:pt x="159298" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3528,8 +4352,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3645556" y="511609"/>
-          <a:ext cx="174891" cy="1598067"/>
+          <a:off x="2744334" y="466074"/>
+          <a:ext cx="159298" cy="1455594"/>
         </a:xfrm>
         <a:custGeom>
           <a:avLst/>
@@ -3540,16 +4364,16 @@
           <a:pathLst>
             <a:path>
               <a:moveTo>
-                <a:pt x="0" y="1598067"/>
+                <a:pt x="0" y="1455594"/>
               </a:moveTo>
               <a:lnTo>
-                <a:pt x="87445" y="1598067"/>
+                <a:pt x="79649" y="1455594"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="87445" y="0"/>
+                <a:pt x="79649" y="0"/>
               </a:lnTo>
               <a:lnTo>
-                <a:pt x="174891" y="0"/>
+                <a:pt x="159298" y="0"/>
               </a:lnTo>
             </a:path>
           </a:pathLst>
@@ -3589,8 +4413,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="2771100" y="1976322"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="1947839" y="1800203"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3631,12 +4455,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3648,15 +4472,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>(index)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="2771100" y="1976322"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="1947839" y="1800203"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}">
@@ -3666,8 +4490,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3820447" y="378255"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="2903633" y="344608"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3708,12 +4532,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -3725,15 +4549,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>(survey)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3820447" y="378255"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="2903633" y="344608"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}">
@@ -3743,306 +4567,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4869793" y="2239"/>
-          <a:ext cx="874455" cy="266708"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
-            <a:t>(vote)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4869793" y="2239"/>
-        <a:ext cx="874455" cy="266708"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4869793" y="378255"/>
-          <a:ext cx="874455" cy="266708"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
-            <a:t>regist</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4869793" y="378255"/>
-        <a:ext cx="874455" cy="266708"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4869793" y="754271"/>
-          <a:ext cx="874455" cy="266708"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
-            <a:t>view</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4869793" y="754271"/>
-        <a:ext cx="874455" cy="266708"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3820447" y="1506302"/>
-          <a:ext cx="874455" cy="266708"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
-            <a:t>make</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3820447" y="1506302"/>
-        <a:ext cx="874455" cy="266708"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4869793" y="1130286"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="3859427" y="2116"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4102,12 +4628,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4119,26 +4645,26 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
-            <a:t>check</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>vote</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4869793" y="1130286"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="3859427" y="2116"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
+    <dsp:sp modelId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4869793" y="1506302"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="3859427" y="344608"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4148,7 +4674,7 @@
         </a:solidFill>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="accent5"/>
+            <a:schemeClr val="accent6"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
@@ -4156,25 +4682,25 @@
       </dsp:spPr>
       <dsp:style>
         <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
+          <a:schemeClr val="accent6"/>
         </a:lnRef>
         <a:fillRef idx="1">
           <a:schemeClr val="lt1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
+          <a:schemeClr val="accent6"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="dk1"/>
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4186,26 +4712,103 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>regist</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4869793" y="1506302"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="3859427" y="344608"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
+    <dsp:sp modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4869793" y="1882318"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="3859427" y="687101"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>(view)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3859427" y="687101"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2903633" y="1372087"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4265,12 +4868,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4282,15 +4885,274 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
-            <a:t>end</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>make</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4869793" y="1882318"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="2903633" y="1372087"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3859427" y="1029594"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent3">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="accent3">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent3">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>check</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3859427" y="1029594"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3859427" y="1372087"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent3"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>regist</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3859427" y="1372087"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3859427" y="1714580"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent3">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="accent3">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent3">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>end</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3859427" y="1714580"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
@@ -4300,8 +5162,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3820447" y="1882318"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="2903633" y="2057073"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4361,12 +5223,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4378,15 +5240,111 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>my(page)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3820447" y="1882318"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="2903633" y="2057073"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{B364BDD2-2468-482C-B4F5-1A0AB60AF7B9}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3859427" y="2057073"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="accent5">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="accent5">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="accent5">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent5">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>fav(orite)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3859427" y="2057073"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
@@ -4396,8 +5354,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3820447" y="2446342"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="2903633" y="2570812"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4428,12 +5386,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4445,15 +5403,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>auth</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3820447" y="2446342"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="2903633" y="2570812"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
@@ -4463,8 +5421,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4869793" y="2258334"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="3859427" y="2399565"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4495,12 +5453,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4512,15 +5470,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>(login)</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4869793" y="2258334"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="3859427" y="2399565"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
@@ -4530,8 +5488,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="4869793" y="2634350"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="3859427" y="2742058"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4562,12 +5520,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4579,15 +5537,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>logout</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="4869793" y="2634350"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="3859427" y="2742058"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
@@ -4597,8 +5555,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3820447" y="2822358"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="2903633" y="2913305"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4639,12 +5597,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4656,15 +5614,15 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>tag</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3820447" y="2822358"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="2903633" y="2913305"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
@@ -4674,8 +5632,8 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3820447" y="3198373"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="2903633" y="3255798"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4716,12 +5674,12 @@
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4733,45 +5691,37 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
             <a:t>user</a:t>
           </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3820447" y="3198373"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="2903633" y="3255798"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
-    <dsp:sp modelId="{0FAB1775-08F8-482E-A204-647B49CA8593}">
+    <dsp:sp modelId="{29399504-D2C7-4F6F-AF1C-8ACC2C7B5F96}">
       <dsp:nvSpPr>
         <dsp:cNvPr id="0" name=""/>
         <dsp:cNvSpPr/>
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm>
-          <a:off x="3820447" y="3574389"/>
-          <a:ext cx="874455" cy="266708"/>
+          <a:off x="1947839" y="3598290"/>
+          <a:ext cx="796494" cy="242930"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
+          <a:schemeClr val="dk1"/>
         </a:solidFill>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
+            <a:schemeClr val="dk1">
+              <a:shade val="50000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
@@ -4780,25 +5730,27 @@
       </dsp:spPr>
       <dsp:style>
         <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:schemeClr val="dk1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
         </a:lnRef>
         <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:schemeClr val="dk1"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:schemeClr val="dk1"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="lt1"/>
         </a:fontRef>
       </dsp:style>
       <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="10795" tIns="10795" rIns="10795" bIns="10795" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
           <a:noAutofit/>
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="755650">
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -4810,15 +5762,320 @@
             </a:spcAft>
           </a:pPr>
           <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1700" kern="1200"/>
-            <a:t>favorite</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1700" kern="1200"/>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>view</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm>
-        <a:off x="3820447" y="3574389"/>
-        <a:ext cx="874455" cy="266708"/>
+        <a:off x="1947839" y="3598290"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{8D36FDD9-C4A3-439F-8065-9CD5119A8A1D}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="2903633" y="3598290"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="dk1">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="dk1">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="dk1">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="38000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>userOnly</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="2903633" y="3598290"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{E167FCA0-7961-4302-99E1-B15A3C1C0377}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3859427" y="3598290"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="dk1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>notView</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3859427" y="3598290"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{3AD42AA0-D75A-4389-96E7-C60023E6261B}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="4815221" y="3598290"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>hideTarget</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="4815221" y="3598290"/>
+        <a:ext cx="796494" cy="242930"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{2D16E66E-9349-4E5D-B7C0-3011230746DB}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5771015" y="3598290"/>
+          <a:ext cx="796494" cy="242930"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent3"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent3">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent3">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent3"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent3"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+          </a:pPr>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
+            <a:t>notDirect</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="5771015" y="3598290"/>
+        <a:ext cx="796494" cy="242930"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -8194,8 +9451,8 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8205,7 +9462,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9963150" y="361950"/>
-          <a:ext cx="7591425" cy="6600825"/>
+          <a:ext cx="7591425" cy="7610475"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8920,8 +10177,21 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
-            <a:t>項目１に投票しました！</a:t>
-          </a:r>
+            <a:t>項目１に投票しました！投票タイトル</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" baseline="0"/>
+            <a:t>tohyomaker.com/20  #tohyomaker</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -8929,16 +10199,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -8947,8 +10217,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="14449425" y="4600575"/>
-          <a:ext cx="1019175" cy="476250"/>
+          <a:off x="10401300" y="5895975"/>
+          <a:ext cx="5095875" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -8990,14 +10260,14 @@
     <xdr:from>
       <xdr:col>15</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -9006,7 +10276,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10372725" y="5457825"/>
+          <a:off x="10372725" y="6648450"/>
           <a:ext cx="5095875" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -9034,7 +10304,7 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
-            <a:t>結果ページ</a:t>
+            <a:t>投票ページへ</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -9045,61 +10315,6 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>352425</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="テキスト ボックス 49"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="1038225" y="4600575"/>
-          <a:ext cx="5095875" cy="476250"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln w="3175"/>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
-            <a:t>何かコメントをつける</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
       <xdr:row>26</xdr:row>
       <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
@@ -9116,8 +10331,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3619501" y="4600575"/>
-          <a:ext cx="2495550" cy="476250"/>
+          <a:off x="1038225" y="4600575"/>
+          <a:ext cx="5076826" cy="476250"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -9323,8 +10538,9 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400"/>
-            <a:t>結果ページ</a:t>
-          </a:r>
+            <a:t>結果ページへ</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -14381,8 +15597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -14413,7 +15629,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
       <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
create helper update survey/vote copy to clipboard module -> todo
</commit_message>
<xml_diff>
--- a/view_plan.xlsx
+++ b/view_plan.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>あ</t>
     <phoneticPr fontId="1"/>
@@ -32,6 +32,38 @@
   </si>
   <si>
     <t>title</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>is_vote</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>select</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>isset</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>btn-info</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>btn-info active</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>jj</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>add_class</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2454,6 +2486,13 @@
     <dgm:pt modelId="{1A2B8F52-9746-463C-BC4A-04A1B691DD53}" type="pres">
       <dgm:prSet presAssocID="{5D3DE17C-EE5A-47BA-A905-F53770A94AE5}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="6" presStyleCnt="10"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{9F313496-2623-4AFE-A6FB-DA38AFC23721}" type="pres">
       <dgm:prSet presAssocID="{A1986176-DBC3-405D-9BBF-0DA05F670219}" presName="hierRoot2" presStyleCnt="0">
@@ -2839,6 +2878,13 @@
     <dgm:pt modelId="{525C1C18-1E95-47D9-936A-CDC62511FB07}" type="pres">
       <dgm:prSet presAssocID="{C10D3E82-F9A1-462C-8FBA-5BD8E7806F8E}" presName="Name64" presStyleLbl="parChTrans1D2" presStyleIdx="6" presStyleCnt="7"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{5A5AF78F-94BC-4F72-B04B-AA02D9CABE93}" type="pres">
       <dgm:prSet presAssocID="{FA6FF089-541E-4496-A510-F6D4516B2FC8}" presName="hierRoot2" presStyleCnt="0">
@@ -2885,6 +2931,13 @@
     <dgm:pt modelId="{7ABFFC0D-740C-4B29-AD4D-33E87F0E3ADD}" type="pres">
       <dgm:prSet presAssocID="{D6DCACAB-7D92-46B6-A2ED-8043909D48F3}" presName="Name64" presStyleLbl="parChTrans1D3" presStyleIdx="9" presStyleCnt="10"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{98628486-4CE5-4842-B931-3C49C481B35B}" type="pres">
       <dgm:prSet presAssocID="{0FE1D759-A2B0-4446-9D87-B95385F80179}" presName="hierRoot2" presStyleCnt="0">
@@ -2931,6 +2984,13 @@
     <dgm:pt modelId="{5A3D3ADE-65DD-4A97-9D37-14548E59672B}" type="pres">
       <dgm:prSet presAssocID="{DA47D477-365A-4A74-AA96-5E5FEB632109}" presName="Name64" presStyleLbl="parChTrans1D4" presStyleIdx="0" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{B33B3A64-A2D1-4FDF-95D1-18EE677C1D5B}" type="pres">
       <dgm:prSet presAssocID="{21CCE5FE-9025-43CD-A96F-F7E3D2ADAB65}" presName="hierRoot2" presStyleCnt="0">
@@ -2977,6 +3037,13 @@
     <dgm:pt modelId="{378BE822-37E6-4E09-9C01-8504E675B5C7}" type="pres">
       <dgm:prSet presAssocID="{B2F685BA-1AC9-4C10-A5F5-3E7531009405}" presName="Name64" presStyleLbl="parChTrans1D4" presStyleIdx="1" presStyleCnt="2"/>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{5AF27C3A-2C7A-4CEF-8400-0C492FA94EDD}" type="pres">
       <dgm:prSet presAssocID="{B27AFB5B-AF36-4250-86F7-A5CBF0A00F27}" presName="hierRoot2" presStyleCnt="0">
@@ -3289,2795 +3356,6 @@
       <dsp:cNvGrpSpPr/>
     </dsp:nvGrpSpPr>
     <dsp:grpSpPr/>
-    <dsp:sp modelId="{378BE822-37E6-4E09-9C01-8504E675B5C7}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5611716" y="3674036"/>
-          <a:ext cx="159298" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="159298" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{5A3D3ADE-65DD-4A97-9D37-14548E59672B}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4655922" y="3674036"/>
-          <a:ext cx="159298" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="159298" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{7ABFFC0D-740C-4B29-AD4D-33E87F0E3ADD}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="3674036"/>
-          <a:ext cx="159298" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="159298" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{525C1C18-1E95-47D9-936A-CDC62511FB07}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2744334" y="3674036"/>
-          <a:ext cx="159298" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="159298" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{400A970B-01E2-495E-9ECB-7EADDBB33666}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2744334" y="1921669"/>
-          <a:ext cx="159298" cy="1455594"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="1455594"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="1455594"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{FAB5C5E7-628B-4269-AFDB-5443D44E7D07}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2744334" y="1921669"/>
-          <a:ext cx="159298" cy="1113101"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="1113101"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="1113101"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{94834600-2A81-4D2E-BA8C-D171F42E9531}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="2692277"/>
-          <a:ext cx="159298" cy="171246"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="171246"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="171246"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{AA914339-50E6-41A3-BF3B-85A6586BBBDD}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="2521031"/>
-          <a:ext cx="159298" cy="171246"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="171246"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="171246"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{E0568980-BD26-44B0-99C5-2B5582E6C423}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2744334" y="1921669"/>
-          <a:ext cx="159298" cy="770608"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="770608"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="770608"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{1A2B8F52-9746-463C-BC4A-04A1B691DD53}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="2132818"/>
-          <a:ext cx="159298" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="159298" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{8FFFBC32-6481-419C-BB5C-77D1F2435B4C}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2744334" y="1921669"/>
-          <a:ext cx="159298" cy="256869"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="256869"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="256869"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{B5C7155C-B21A-4598-BDC2-8EF762D049C0}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="1493552"/>
-          <a:ext cx="159298" cy="342492"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="342492"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="342492"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{224BDC60-7934-422F-B29C-84F028B56716}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="1447832"/>
-          <a:ext cx="159298" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="159298" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{6390FF4A-F0A9-4F65-975E-14F195A61516}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="1151060"/>
-          <a:ext cx="159298" cy="342492"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="342492"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="342492"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{FF665FCC-0648-4557-B7F6-8C6B70F83736}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2744334" y="1493552"/>
-          <a:ext cx="159298" cy="428116"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="428116"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="428116"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{1B49C5E6-75F6-41DB-AF44-C9451B868BC9}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="466074"/>
-          <a:ext cx="159298" cy="342492"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="0"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="342492"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="342492"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{A86A5C7B-5BE2-49C4-AF4C-4E4539AFE633}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="420354"/>
-          <a:ext cx="159298" cy="91440"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="45720"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="159298" y="45720"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{12C9F87A-ECA2-4013-907C-A00079EE41ED}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3700128" y="123581"/>
-          <a:ext cx="159298" cy="342492"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="342492"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="342492"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="80000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{9451D74F-6692-4FF1-A580-5574CD4401DB}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2744334" y="466074"/>
-          <a:ext cx="159298" cy="1455594"/>
-        </a:xfrm>
-        <a:custGeom>
-          <a:avLst/>
-          <a:gdLst/>
-          <a:ahLst/>
-          <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
-          <a:pathLst>
-            <a:path>
-              <a:moveTo>
-                <a:pt x="0" y="1455594"/>
-              </a:moveTo>
-              <a:lnTo>
-                <a:pt x="79649" y="1455594"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="79649" y="0"/>
-              </a:lnTo>
-              <a:lnTo>
-                <a:pt x="159298" y="0"/>
-              </a:lnTo>
-            </a:path>
-          </a:pathLst>
-        </a:custGeom>
-        <a:noFill/>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent1">
-              <a:shade val="60000"/>
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor"/>
-      </dsp:style>
-    </dsp:sp>
-    <dsp:sp modelId="{7982B9D9-F4CA-4526-AF01-1C66846C2247}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1947839" y="1800203"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>(index)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="1947839" y="1800203"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{49B2B401-190F-48F3-9418-BF5302A3E8E7}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2903633" y="344608"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>(survey)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2903633" y="344608"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{C4F35D36-C001-4B0D-B4A0-9B8733C273C8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="2116"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="accent5">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="accent5">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent5">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>vote</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="2116"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{E4DB054B-0D42-43B5-8068-D3D5661AF0CB}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="344608"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>regist</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="344608"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8BF43C11-C06B-4E7D-8F41-50A19E6FD729}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="687101"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>(view)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="687101"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8468714C-BAA1-4E65-AD30-004F9F01A6CF}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2903633" y="1372087"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="accent5">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="accent5">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent5">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>make</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2903633" y="1372087"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{3323E5C0-8F57-4DBF-917A-B8F500CCD3B3}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="1029594"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="accent3">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="accent3">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent3">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>check</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="1029594"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{7B940FB6-79A9-43AD-AAD0-E00D6181EE77}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="1372087"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent3"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>regist</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="1372087"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{EFEF81FB-55BB-4A5C-ACB3-7B2D9728F7C6}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="1714580"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="accent3">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="accent3">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent3">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>end</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="1714580"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{A2CCD8F7-BF82-4CF1-82C0-4DECA47B2E8C}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2903633" y="2057073"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="accent5">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="accent5">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent5">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>my(page)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2903633" y="2057073"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{B364BDD2-2468-482C-B4F5-1A0AB60AF7B9}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="2057073"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="accent5">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="accent5">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="accent5">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>fav(orite)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="2057073"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F2F19CDA-76D5-4F9F-92B9-0CEC8982C764}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2903633" y="2570812"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>auth</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2903633" y="2570812"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{930B9FC5-A78E-4242-AA74-C65A4D8DE2D4}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="2399565"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>(login)</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="2399565"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{F5B18884-E498-499B-92AD-14DA40157B0A}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="2742058"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent5"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent5"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent5"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>logout</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="2742058"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{609F8005-8F5B-42D4-A2E8-650C5639BED8}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2903633" y="2913305"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>tag</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2903633" y="2913305"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{40DF2346-36E7-4A3C-9F1E-B8BB7FA9557E}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2903633" y="3255798"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent1">
-            <a:hueOff val="0"/>
-            <a:satOff val="0"/>
-            <a:lumOff val="0"/>
-            <a:alphaOff val="0"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="lt1">
-              <a:hueOff val="0"/>
-              <a:satOff val="0"/>
-              <a:lumOff val="0"/>
-              <a:alphaOff val="0"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>user</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2903633" y="3255798"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{29399504-D2C7-4F6F-AF1C-8ACC2C7B5F96}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="1947839" y="3598290"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="dk1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>view</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="1947839" y="3598290"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{8D36FDD9-C4A3-439F-8065-9CD5119A8A1D}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="2903633" y="3598290"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="dk1">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="dk1">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="dk1">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst>
-          <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-            <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>userOnly</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="2903633" y="3598290"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{E167FCA0-7961-4302-99E1-B15A3C1C0377}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="3859427" y="3598290"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="lt1"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="dk1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="lt1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="dk1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>notView</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="3859427" y="3598290"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{3AD42AA0-D75A-4389-96E7-C60023E6261B}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="4815221" y="3598290"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent6"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent6">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent6">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>hideTarget</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="4815221" y="3598290"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
-    <dsp:sp modelId="{2D16E66E-9349-4E5D-B7C0-3011230746DB}">
-      <dsp:nvSpPr>
-        <dsp:cNvPr id="0" name=""/>
-        <dsp:cNvSpPr/>
-      </dsp:nvSpPr>
-      <dsp:spPr>
-        <a:xfrm>
-          <a:off x="5771015" y="3598290"/>
-          <a:ext cx="796494" cy="242930"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="accent3"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="accent3">
-              <a:shade val="50000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:effectLst/>
-      </dsp:spPr>
-      <dsp:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent3">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent3"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent3"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </dsp:style>
-      <dsp:txBody>
-        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="8890" tIns="8890" rIns="8890" bIns="8890" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
-          <a:noAutofit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr lvl="0" algn="ctr" defTabSz="622300">
-            <a:lnSpc>
-              <a:spcPct val="90000"/>
-            </a:lnSpc>
-            <a:spcBef>
-              <a:spcPct val="0"/>
-            </a:spcBef>
-            <a:spcAft>
-              <a:spcPct val="35000"/>
-            </a:spcAft>
-          </a:pPr>
-          <a:r>
-            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1400" kern="1200"/>
-            <a:t>notDirect</a:t>
-          </a:r>
-          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1400" kern="1200"/>
-        </a:p>
-      </dsp:txBody>
-      <dsp:txXfrm>
-        <a:off x="5771015" y="3598290"/>
-        <a:ext cx="796494" cy="242930"/>
-      </dsp:txXfrm>
-    </dsp:sp>
   </dsp:spTree>
 </dsp:drawing>
 </file>
@@ -10414,15 +7692,9 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200"/>
-            <a:t>投票</a:t>
+            <a:t>未投票</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200"/>
-            <a:t>ページ</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -10476,15 +7748,9 @@
         <a:p>
           <a:r>
             <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200"/>
-            <a:t>投票</a:t>
+            <a:t>投票済み</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1200"/>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1200"/>
-            <a:t>ページ</a:t>
-          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -15627,14 +12893,64 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B43:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I7" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="43" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>4</v>
+      </c>
+      <c r="D43" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B44" t="b">
+        <v>0</v>
+      </c>
+      <c r="C44" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B45" t="b">
+        <v>0</v>
+      </c>
+      <c r="C45" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" x14ac:dyDescent="0.15">
+      <c r="B46" t="b">
+        <v>1</v>
+      </c>
+      <c r="C46" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.15">
+      <c r="D49" t="s">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>